<commit_message>
Transportation sector calibration and redesignating passenger ships as taxis
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\trans\AVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683937AB-F5C5-49F8-95B7-31920D8FD88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="10" yWindow="260" windowWidth="19190" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="India Data" sheetId="12" r:id="rId2"/>
     <sheet name="AVL" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
   <si>
     <t>ships</t>
   </si>
@@ -227,12 +231,15 @@
   </si>
   <si>
     <t>Public Private share of Passenger Km in Road Transport</t>
+  </si>
+  <si>
+    <t>For India, passenger ships are repurposed as taxis.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="17">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2692,7 +2699,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2706,7 +2713,6 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="33" fillId="36" borderId="21" xfId="576" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2777,710 +2783,712 @@
     <xf numFmtId="0" fontId="102" fillId="65" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="702">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="227"/>
-    <cellStyle name="20% - Accent1 3" xfId="385"/>
-    <cellStyle name="20% - Accent1 4" xfId="389"/>
-    <cellStyle name="20% - Accent1 5" xfId="403"/>
+    <cellStyle name="20% - Accent1 2" xfId="227" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="385" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent1 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent1 5" xfId="403" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="20% - Accent2" xfId="37" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="391"/>
-    <cellStyle name="20% - Accent2 3" xfId="405"/>
-    <cellStyle name="20% - Accent2 4" xfId="366"/>
+    <cellStyle name="20% - Accent2 2" xfId="391" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Accent2 3" xfId="405" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent2 4" xfId="366" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="20% - Accent3" xfId="41" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="393"/>
-    <cellStyle name="20% - Accent3 3" xfId="407"/>
-    <cellStyle name="20% - Accent3 4" xfId="370"/>
+    <cellStyle name="20% - Accent3 2" xfId="393" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent3 3" xfId="407" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - Accent3 4" xfId="370" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="20% - Accent4" xfId="45" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="395"/>
-    <cellStyle name="20% - Accent4 3" xfId="409"/>
-    <cellStyle name="20% - Accent4 4" xfId="374"/>
+    <cellStyle name="20% - Accent4 2" xfId="395" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - Accent4 3" xfId="409" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - Accent4 4" xfId="374" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="20% - Accent5" xfId="49" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="397"/>
-    <cellStyle name="20% - Accent5 3" xfId="411"/>
-    <cellStyle name="20% - Accent5 4" xfId="378"/>
+    <cellStyle name="20% - Accent5 2" xfId="397" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - Accent5 3" xfId="411" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - Accent5 4" xfId="378" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="20% - Accent6" xfId="53" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 10" xfId="590"/>
-    <cellStyle name="20% - Accent6 2" xfId="117"/>
-    <cellStyle name="20% - Accent6 3" xfId="344"/>
-    <cellStyle name="20% - Accent6 3 2" xfId="556"/>
-    <cellStyle name="20% - Accent6 4" xfId="347"/>
-    <cellStyle name="20% - Accent6 4 2" xfId="418"/>
-    <cellStyle name="20% - Accent6 5" xfId="386"/>
-    <cellStyle name="20% - Accent6 6" xfId="399"/>
-    <cellStyle name="20% - Accent6 7" xfId="413"/>
-    <cellStyle name="20% - Accent6 8" xfId="559"/>
-    <cellStyle name="20% - Accent6 9" xfId="578"/>
-    <cellStyle name="20% - Colore 1" xfId="424"/>
-    <cellStyle name="20% - Colore 2" xfId="425"/>
-    <cellStyle name="20% - Colore 3" xfId="426"/>
-    <cellStyle name="20% - Colore 4" xfId="427"/>
-    <cellStyle name="20% - Colore 5" xfId="428"/>
-    <cellStyle name="20% - Colore 6" xfId="429"/>
+    <cellStyle name="20% - Accent6 10" xfId="590" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - Accent6 3" xfId="344" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="20% - Accent6 3 2" xfId="556" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="20% - Accent6 4" xfId="347" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="20% - Accent6 4 2" xfId="418" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - Accent6 5" xfId="386" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="20% - Accent6 6" xfId="399" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Accent6 7" xfId="413" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="20% - Accent6 8" xfId="559" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="20% - Accent6 9" xfId="578" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="20% - Colore 1" xfId="424" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="20% - Colore 2" xfId="425" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="20% - Colore 3" xfId="426" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - Colore 4" xfId="427" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="20% - Colore 5" xfId="428" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - Colore 6" xfId="429" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="40% - Accent1" xfId="34" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="390"/>
-    <cellStyle name="40% - Accent1 3" xfId="404"/>
-    <cellStyle name="40% - Accent1 4" xfId="363"/>
+    <cellStyle name="40% - Accent1 2" xfId="390" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="40% - Accent1 3" xfId="404" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="40% - Accent1 4" xfId="363" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="40% - Accent2" xfId="38" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="392"/>
-    <cellStyle name="40% - Accent2 3" xfId="406"/>
-    <cellStyle name="40% - Accent2 4" xfId="367"/>
+    <cellStyle name="40% - Accent2 2" xfId="392" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="40% - Accent2 3" xfId="406" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="40% - Accent2 4" xfId="367" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="40% - Accent3" xfId="42" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="394"/>
-    <cellStyle name="40% - Accent3 3" xfId="408"/>
-    <cellStyle name="40% - Accent3 4" xfId="371"/>
+    <cellStyle name="40% - Accent3 2" xfId="394" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="40% - Accent3 3" xfId="408" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="40% - Accent3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="40% - Accent4" xfId="46" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="396"/>
-    <cellStyle name="40% - Accent4 3" xfId="410"/>
-    <cellStyle name="40% - Accent4 4" xfId="375"/>
+    <cellStyle name="40% - Accent4 2" xfId="396" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="40% - Accent4 3" xfId="410" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="40% - Accent4 4" xfId="375" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="40% - Accent5" xfId="50" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="398"/>
-    <cellStyle name="40% - Accent5 3" xfId="412"/>
-    <cellStyle name="40% - Accent5 4" xfId="379"/>
+    <cellStyle name="40% - Accent5 2" xfId="398" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="40% - Accent5 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="40% - Accent5 4" xfId="379" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
     <cellStyle name="40% - Accent6" xfId="54" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="400"/>
-    <cellStyle name="40% - Accent6 3" xfId="414"/>
-    <cellStyle name="40% - Accent6 4" xfId="381"/>
-    <cellStyle name="40% - Colore 1" xfId="430"/>
-    <cellStyle name="40% - Colore 2" xfId="431"/>
-    <cellStyle name="40% - Colore 3" xfId="432"/>
-    <cellStyle name="40% - Colore 4" xfId="433"/>
-    <cellStyle name="40% - Colore 5" xfId="434"/>
-    <cellStyle name="40% - Colore 6" xfId="435"/>
+    <cellStyle name="40% - Accent6 2" xfId="400" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="40% - Accent6 3" xfId="414" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="40% - Accent6 4" xfId="381" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="40% - Colore 1" xfId="430" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="40% - Colore 2" xfId="431" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="40% - Colore 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="40% - Colore 4" xfId="433" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="40% - Colore 5" xfId="434" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="40% - Colore 6" xfId="435" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
     <cellStyle name="60% - Accent1" xfId="35" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1 2" xfId="364"/>
+    <cellStyle name="60% - Accent1 2" xfId="364" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
     <cellStyle name="60% - Accent2" xfId="39" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2 2" xfId="368"/>
+    <cellStyle name="60% - Accent2 2" xfId="368" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="60% - Accent3" xfId="43" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3 2" xfId="372"/>
+    <cellStyle name="60% - Accent3 2" xfId="372" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
     <cellStyle name="60% - Accent4" xfId="47" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4 2" xfId="376"/>
+    <cellStyle name="60% - Accent4 2" xfId="376" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
     <cellStyle name="60% - Accent5" xfId="51" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5 2" xfId="380"/>
+    <cellStyle name="60% - Accent5 2" xfId="380" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
     <cellStyle name="60% - Accent6" xfId="55" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6 2" xfId="382"/>
-    <cellStyle name="60% - Colore 1" xfId="436"/>
-    <cellStyle name="60% - Colore 2" xfId="437"/>
-    <cellStyle name="60% - Colore 3" xfId="438"/>
-    <cellStyle name="60% - Colore 4" xfId="439"/>
-    <cellStyle name="60% - Colore 5" xfId="440"/>
-    <cellStyle name="60% - Colore 6" xfId="441"/>
-    <cellStyle name="A - a heading" xfId="581"/>
-    <cellStyle name="A - bold" xfId="584"/>
-    <cellStyle name="A - bottom border" xfId="586"/>
-    <cellStyle name="A - bottom border 2" xfId="701"/>
-    <cellStyle name="A - header" xfId="583"/>
-    <cellStyle name="A - header 2" xfId="598"/>
-    <cellStyle name="A - header 2 2" xfId="602"/>
-    <cellStyle name="A - normal" xfId="582"/>
-    <cellStyle name="A - percent" xfId="587"/>
+    <cellStyle name="60% - Accent6 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="60% - Colore 1" xfId="436" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="60% - Colore 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="60% - Colore 3" xfId="438" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="60% - Colore 4" xfId="439" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="60% - Colore 5" xfId="440" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="60% - Colore 6" xfId="441" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="A - a heading" xfId="581" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="A - bold" xfId="584" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="A - bottom border" xfId="586" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="A - bottom border 2" xfId="701" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="A - header" xfId="583" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="A - header 2" xfId="598" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="A - header 2 2" xfId="602" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="A - normal" xfId="582" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="A - percent" xfId="587" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
     <cellStyle name="Accent1" xfId="32" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 2" xfId="362"/>
+    <cellStyle name="Accent1 2" xfId="362" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
     <cellStyle name="Accent2" xfId="36" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="365"/>
+    <cellStyle name="Accent2 2" xfId="365" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
     <cellStyle name="Accent3" xfId="40" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="369"/>
+    <cellStyle name="Accent3 2" xfId="369" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
     <cellStyle name="Accent4" xfId="44" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="373"/>
+    <cellStyle name="Accent4 2" xfId="373" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
     <cellStyle name="Accent5" xfId="48" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="377"/>
+    <cellStyle name="Accent5 2" xfId="377" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
     <cellStyle name="Accent6" xfId="52" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="348"/>
+    <cellStyle name="Accent6 2" xfId="348" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
     <cellStyle name="Bad" xfId="21" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="353"/>
-    <cellStyle name="Best" xfId="442"/>
-    <cellStyle name="Body: normal cell" xfId="2"/>
-    <cellStyle name="BORDERS" xfId="443"/>
-    <cellStyle name="BORDERS 2" xfId="444"/>
-    <cellStyle name="BORDERS 2 2" xfId="679"/>
-    <cellStyle name="BORDERS 3" xfId="678"/>
-    <cellStyle name="Calc Currency (0)" xfId="445"/>
-    <cellStyle name="Calcolo" xfId="446"/>
-    <cellStyle name="Calcolo 2" xfId="447"/>
-    <cellStyle name="Calcolo 2 2" xfId="681"/>
-    <cellStyle name="Calcolo 3" xfId="448"/>
-    <cellStyle name="Calcolo 3 2" xfId="682"/>
-    <cellStyle name="Calcolo 4" xfId="680"/>
+    <cellStyle name="Bad 2" xfId="353" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Best" xfId="442" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="BORDERS" xfId="443" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="BORDERS 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="BORDERS 2 2" xfId="679" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="BORDERS 3" xfId="678" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Calc Currency (0)" xfId="445" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Calcolo" xfId="446" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Calcolo 2" xfId="447" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Calcolo 2 2" xfId="681" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Calcolo 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Calcolo 3 2" xfId="682" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Calcolo 4" xfId="680" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
     <cellStyle name="Calculation" xfId="25" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Calculation 2" xfId="356"/>
-    <cellStyle name="Cella collegata" xfId="449"/>
-    <cellStyle name="Cella da controllare" xfId="450"/>
+    <cellStyle name="Calculation 2" xfId="356" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Cella collegata" xfId="449" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Cella da controllare" xfId="450" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Check Cell 2" xfId="358"/>
-    <cellStyle name="Colore 1" xfId="451"/>
-    <cellStyle name="Colore 2" xfId="452"/>
-    <cellStyle name="Colore 3" xfId="453"/>
-    <cellStyle name="Colore 4" xfId="454"/>
-    <cellStyle name="Colore 5" xfId="455"/>
-    <cellStyle name="Colore 6" xfId="456"/>
-    <cellStyle name="Column - Style5" xfId="457"/>
-    <cellStyle name="Column - Style6" xfId="458"/>
-    <cellStyle name="Column headings" xfId="459"/>
-    <cellStyle name="Column headings 2" xfId="683"/>
-    <cellStyle name="Comma 2" xfId="230"/>
-    <cellStyle name="Comma 2 2" xfId="460"/>
-    <cellStyle name="Comma 2 3" xfId="420"/>
-    <cellStyle name="Comma 2 4" xfId="573"/>
-    <cellStyle name="Comma 3" xfId="416"/>
-    <cellStyle name="Comma 3 2" xfId="462"/>
-    <cellStyle name="Comma 3 3" xfId="461"/>
-    <cellStyle name="Comma 4" xfId="463"/>
-    <cellStyle name="Comma 4 2" xfId="562"/>
-    <cellStyle name="Comma 5" xfId="464"/>
-    <cellStyle name="Comma 6" xfId="422"/>
-    <cellStyle name="Comma 7" xfId="579"/>
-    <cellStyle name="Comma 8" xfId="589"/>
-    <cellStyle name="Comma 9" xfId="62"/>
-    <cellStyle name="Comma0" xfId="465"/>
-    <cellStyle name="Copied" xfId="466"/>
-    <cellStyle name="Currency 2" xfId="557"/>
-    <cellStyle name="Currency0" xfId="467"/>
-    <cellStyle name="Data" xfId="13"/>
-    <cellStyle name="Data (Number)" xfId="468"/>
-    <cellStyle name="Data (Text)" xfId="469"/>
-    <cellStyle name="Data no deci" xfId="59"/>
-    <cellStyle name="Date" xfId="470"/>
-    <cellStyle name="Entered" xfId="471"/>
-    <cellStyle name="Excel Built-in Normal" xfId="114"/>
+    <cellStyle name="Check Cell 2" xfId="358" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Colore 1" xfId="451" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Colore 2" xfId="452" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Colore 3" xfId="453" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Colore 4" xfId="454" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Colore 5" xfId="455" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Colore 6" xfId="456" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Column - Style5" xfId="457" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Column - Style6" xfId="458" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Column headings" xfId="459" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Column headings 2" xfId="683" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Comma 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Comma 2 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Comma 2 3" xfId="420" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Comma 2 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Comma 3" xfId="416" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Comma 3 2" xfId="462" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Comma 3 3" xfId="461" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Comma 4" xfId="463" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Comma 4 2" xfId="562" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Comma 5" xfId="464" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Comma 6" xfId="422" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Comma 7" xfId="579" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Comma 8" xfId="589" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Comma 9" xfId="62" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Comma0" xfId="465" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Copied" xfId="466" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Currency 2" xfId="557" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Currency0" xfId="467" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Data" xfId="13" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Data (Number)" xfId="468" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Data (Text)" xfId="469" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Data no deci" xfId="59" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Date" xfId="470" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Entered" xfId="471" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="114" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
     <cellStyle name="Explanatory Text" xfId="30" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="360"/>
-    <cellStyle name="FIGURES" xfId="472"/>
-    <cellStyle name="Fixed" xfId="473"/>
+    <cellStyle name="Explanatory Text 2" xfId="360" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="FIGURES" xfId="472" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Fixed" xfId="473" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="8"/>
-    <cellStyle name="Footnote Text" xfId="474"/>
-    <cellStyle name="Footnotes: all except top row" xfId="11"/>
-    <cellStyle name="Footnotes: top row" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="8" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Footnote Text" xfId="474" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="11" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
     <cellStyle name="Good" xfId="20" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="343"/>
-    <cellStyle name="Grey" xfId="475"/>
-    <cellStyle name="Header: bottom row" xfId="1"/>
-    <cellStyle name="Header: top rows" xfId="3"/>
-    <cellStyle name="Header1" xfId="476"/>
-    <cellStyle name="Header2" xfId="477"/>
-    <cellStyle name="Header2 2" xfId="478"/>
-    <cellStyle name="Header2 2 2" xfId="685"/>
-    <cellStyle name="Header2 3" xfId="479"/>
-    <cellStyle name="Header2 3 2" xfId="686"/>
-    <cellStyle name="Header2 4" xfId="684"/>
+    <cellStyle name="Good 2" xfId="343" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Grey" xfId="475" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Header: bottom row" xfId="1" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Header: top rows" xfId="3" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Header1" xfId="476" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Header2" xfId="477" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Header2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Header2 2 2" xfId="685" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Header2 3" xfId="479" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Header2 3 2" xfId="686" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Header2 4" xfId="684" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
     <cellStyle name="Heading 1" xfId="16" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 1 2" xfId="349"/>
+    <cellStyle name="Heading 1 2" xfId="349" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
     <cellStyle name="Heading 2" xfId="17" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 2 2" xfId="350"/>
+    <cellStyle name="Heading 2 2" xfId="350" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
     <cellStyle name="Heading 3" xfId="18" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 3 2" xfId="351"/>
+    <cellStyle name="Heading 3 2" xfId="351" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
     <cellStyle name="Heading 4" xfId="19" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Heading 4 2" xfId="352"/>
-    <cellStyle name="Hed Side" xfId="14"/>
-    <cellStyle name="Hed Side Regular" xfId="58"/>
-    <cellStyle name="Hed Top" xfId="57"/>
-    <cellStyle name="Hyperlink 10" xfId="125" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="280" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="615"/>
-    <cellStyle name="Hyperlink 100" xfId="215" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="330" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="665"/>
-    <cellStyle name="Hyperlink 101" xfId="216" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="331" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="666"/>
-    <cellStyle name="Hyperlink 102" xfId="217" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="332" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="667"/>
-    <cellStyle name="Hyperlink 103" xfId="218" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="333" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="668"/>
-    <cellStyle name="Hyperlink 104" xfId="219" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="334" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="669"/>
-    <cellStyle name="Hyperlink 105" xfId="220" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="335" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="670"/>
-    <cellStyle name="Hyperlink 106" xfId="221" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="336" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="671"/>
-    <cellStyle name="Hyperlink 107" xfId="222" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="337" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="672"/>
-    <cellStyle name="Hyperlink 108" xfId="223" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="338" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="673"/>
-    <cellStyle name="Hyperlink 109" xfId="224" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="339" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="674"/>
-    <cellStyle name="Hyperlink 11" xfId="126" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="279" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="614"/>
-    <cellStyle name="Hyperlink 110" xfId="225" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="340" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="675"/>
-    <cellStyle name="Hyperlink 111" xfId="226" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="341" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="676"/>
-    <cellStyle name="Hyperlink 112" xfId="555"/>
-    <cellStyle name="Hyperlink 113" xfId="115"/>
-    <cellStyle name="Hyperlink 12" xfId="127" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="278" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="613"/>
-    <cellStyle name="Hyperlink 13" xfId="128" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="277" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="612"/>
-    <cellStyle name="Hyperlink 14" xfId="129" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="276" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="68"/>
-    <cellStyle name="Hyperlink 15" xfId="130" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="275" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="69"/>
-    <cellStyle name="Hyperlink 16" xfId="131" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="274" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="70"/>
-    <cellStyle name="Hyperlink 17" xfId="132" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="273" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="71"/>
-    <cellStyle name="Hyperlink 18" xfId="133" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="272" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="72"/>
-    <cellStyle name="Hyperlink 19" xfId="134" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="271" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="73"/>
-    <cellStyle name="Hyperlink 2" xfId="9"/>
-    <cellStyle name="Hyperlink 2 2" xfId="480"/>
-    <cellStyle name="Hyperlink 2 3" xfId="116" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="228" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="288" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="342" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="113" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="623" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="677"/>
-    <cellStyle name="Hyperlink 20" xfId="135" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="270" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="74"/>
-    <cellStyle name="Hyperlink 21" xfId="136" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="269" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="75"/>
-    <cellStyle name="Hyperlink 22" xfId="137" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="268" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="76"/>
-    <cellStyle name="Hyperlink 23" xfId="138" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="267" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="77"/>
-    <cellStyle name="Hyperlink 24" xfId="139" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="266" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="78"/>
-    <cellStyle name="Hyperlink 25" xfId="140" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="265" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="79"/>
-    <cellStyle name="Hyperlink 26" xfId="141" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="264" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="80"/>
-    <cellStyle name="Hyperlink 27" xfId="142" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="263" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="81"/>
-    <cellStyle name="Hyperlink 28" xfId="143" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="262" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="82"/>
-    <cellStyle name="Hyperlink 29" xfId="144" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="261" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="83"/>
-    <cellStyle name="Hyperlink 3" xfId="118" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="287" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="622"/>
-    <cellStyle name="Hyperlink 30" xfId="145" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="260" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="84"/>
-    <cellStyle name="Hyperlink 31" xfId="146" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="259" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="85"/>
-    <cellStyle name="Hyperlink 32" xfId="147" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="258" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="86"/>
-    <cellStyle name="Hyperlink 33" xfId="148" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="257" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="87"/>
-    <cellStyle name="Hyperlink 34" xfId="149" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="256" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="88"/>
-    <cellStyle name="Hyperlink 35" xfId="150" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="255" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="89"/>
-    <cellStyle name="Hyperlink 36" xfId="151" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="254" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="90"/>
-    <cellStyle name="Hyperlink 37" xfId="152" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="253" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="91"/>
-    <cellStyle name="Hyperlink 38" xfId="153" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="252" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="92"/>
-    <cellStyle name="Hyperlink 39" xfId="154" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="251" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="93"/>
-    <cellStyle name="Hyperlink 4" xfId="119" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="286" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="621"/>
-    <cellStyle name="Hyperlink 40" xfId="155" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="250" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="94"/>
-    <cellStyle name="Hyperlink 41" xfId="156" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="249" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="95"/>
-    <cellStyle name="Hyperlink 42" xfId="157" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="248" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="96"/>
-    <cellStyle name="Hyperlink 43" xfId="158" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="247" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="97"/>
-    <cellStyle name="Hyperlink 44" xfId="159" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="246" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="98"/>
-    <cellStyle name="Hyperlink 45" xfId="160" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="245" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="99"/>
-    <cellStyle name="Hyperlink 46" xfId="161" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="244" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="100"/>
-    <cellStyle name="Hyperlink 47" xfId="162" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="243" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="101"/>
-    <cellStyle name="Hyperlink 48" xfId="163" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="242" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="102"/>
-    <cellStyle name="Hyperlink 49" xfId="164" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="241" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="103"/>
-    <cellStyle name="Hyperlink 5" xfId="120" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="285" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="620"/>
-    <cellStyle name="Hyperlink 50" xfId="165" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="240" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="104"/>
-    <cellStyle name="Hyperlink 51" xfId="166" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="239" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="105"/>
-    <cellStyle name="Hyperlink 52" xfId="167" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="238" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="106"/>
-    <cellStyle name="Hyperlink 53" xfId="168" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="237" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="107"/>
-    <cellStyle name="Hyperlink 54" xfId="169" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="236" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="108"/>
-    <cellStyle name="Hyperlink 55" xfId="170" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="235" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="109"/>
-    <cellStyle name="Hyperlink 56" xfId="171" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="234" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="110"/>
-    <cellStyle name="Hyperlink 57" xfId="172" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="233" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="111"/>
-    <cellStyle name="Hyperlink 58" xfId="173" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="289" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="624"/>
-    <cellStyle name="Hyperlink 59" xfId="174" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="232" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="112"/>
-    <cellStyle name="Hyperlink 6" xfId="121" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="284" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="619"/>
-    <cellStyle name="Hyperlink 60" xfId="175" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="290" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="625"/>
-    <cellStyle name="Hyperlink 61" xfId="176" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="291" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="626"/>
-    <cellStyle name="Hyperlink 62" xfId="177" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="292" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="627"/>
-    <cellStyle name="Hyperlink 63" xfId="178" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="293" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="628"/>
-    <cellStyle name="Hyperlink 64" xfId="179" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="294" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="629"/>
-    <cellStyle name="Hyperlink 65" xfId="180" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="295" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="630"/>
-    <cellStyle name="Hyperlink 66" xfId="181" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="296" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="631"/>
-    <cellStyle name="Hyperlink 67" xfId="182" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="297" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="632"/>
-    <cellStyle name="Hyperlink 68" xfId="183" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="298" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="633"/>
-    <cellStyle name="Hyperlink 69" xfId="184" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="299" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="634"/>
-    <cellStyle name="Hyperlink 7" xfId="122" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="283" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="618"/>
-    <cellStyle name="Hyperlink 70" xfId="185" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="300" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="635"/>
-    <cellStyle name="Hyperlink 71" xfId="186" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="301" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="636"/>
-    <cellStyle name="Hyperlink 72" xfId="187" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="302" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="637"/>
-    <cellStyle name="Hyperlink 73" xfId="188" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="303" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="638"/>
-    <cellStyle name="Hyperlink 74" xfId="189" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="304" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="639"/>
-    <cellStyle name="Hyperlink 75" xfId="190" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="305" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="640"/>
-    <cellStyle name="Hyperlink 76" xfId="191" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="306" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="641"/>
-    <cellStyle name="Hyperlink 77" xfId="192" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="307" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="642"/>
-    <cellStyle name="Hyperlink 78" xfId="193" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="308" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="643"/>
-    <cellStyle name="Hyperlink 79" xfId="194" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="309" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="644"/>
-    <cellStyle name="Hyperlink 8" xfId="123" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="282" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="617"/>
-    <cellStyle name="Hyperlink 80" xfId="195" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="310" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="645"/>
-    <cellStyle name="Hyperlink 81" xfId="196" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="311" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="646"/>
-    <cellStyle name="Hyperlink 82" xfId="197" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="312" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="647"/>
-    <cellStyle name="Hyperlink 83" xfId="198" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="313" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="648"/>
-    <cellStyle name="Hyperlink 84" xfId="199" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="314" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="649"/>
-    <cellStyle name="Hyperlink 85" xfId="200" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="315" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="650"/>
-    <cellStyle name="Hyperlink 86" xfId="201" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="316" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="651"/>
-    <cellStyle name="Hyperlink 87" xfId="202" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="317" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="652"/>
-    <cellStyle name="Hyperlink 88" xfId="203" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="318" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="653"/>
-    <cellStyle name="Hyperlink 89" xfId="204" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="319" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="654"/>
-    <cellStyle name="Hyperlink 9" xfId="124" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="281" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="616"/>
-    <cellStyle name="Hyperlink 90" xfId="205" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="320" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="655"/>
-    <cellStyle name="Hyperlink 91" xfId="206" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="321" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="656"/>
-    <cellStyle name="Hyperlink 92" xfId="207" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="322" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="657"/>
-    <cellStyle name="Hyperlink 93" xfId="208" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="323" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="658"/>
-    <cellStyle name="Hyperlink 94" xfId="209" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="324" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="659"/>
-    <cellStyle name="Hyperlink 95" xfId="210" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="325" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="660"/>
-    <cellStyle name="Hyperlink 96" xfId="211" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="326" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="661"/>
-    <cellStyle name="Hyperlink 97" xfId="212" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="327" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="662"/>
-    <cellStyle name="Hyperlink 98" xfId="213" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="328" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="663"/>
-    <cellStyle name="Hyperlink 99" xfId="214" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="329" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="664"/>
+    <cellStyle name="Heading 4 2" xfId="352" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Hed Side" xfId="14" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="58" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Hed Top" xfId="57" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="125" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="280" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="615" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="215" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="330" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="665" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="216" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="331" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="666" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="217" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="332" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="667" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="218" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="333" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="668" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="219" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="334" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="669" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="220" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="335" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="670" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="221" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="336" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="671" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="222" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="337" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="672" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="223" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="338" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="673" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="224" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="339" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="674" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="126" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="279" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="614" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="225" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="340" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="675" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="226" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="341" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="676" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Hyperlink 112" xfId="555" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Hyperlink 113" xfId="115" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="127" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="278" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="613" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="128" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="277" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="612" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="129" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="276" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="68" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="130" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="275" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="69" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="131" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="274" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="70" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Hyperlink 17" xfId="132" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Hyperlink 17" xfId="273" hidden="1" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Hyperlink 17" xfId="71" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="133" hidden="1" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="272" hidden="1" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="72" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="134" hidden="1" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="271" hidden="1" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="73" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="116" hidden="1" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="228" hidden="1" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="288" hidden="1" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="342" hidden="1" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="113" hidden="1" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="623" hidden="1" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="677" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="135" hidden="1" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="270" hidden="1" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="74" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="136" hidden="1" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="269" hidden="1" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="75" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="137" hidden="1" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="268" hidden="1" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="76" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="138" hidden="1" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="267" hidden="1" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="77" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="139" hidden="1" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="266" hidden="1" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="78" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="140" hidden="1" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="265" hidden="1" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="79" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="141" hidden="1" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="264" hidden="1" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="80" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="142" hidden="1" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="263" hidden="1" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="81" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="143" hidden="1" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="262" hidden="1" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="82" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="144" hidden="1" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="261" hidden="1" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="83" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="118" hidden="1" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="287" hidden="1" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="622" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="145" hidden="1" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="260" hidden="1" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="84" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="146" hidden="1" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="259" hidden="1" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="85" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="147" hidden="1" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="258" hidden="1" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="86" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="148" hidden="1" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="257" hidden="1" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="87" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="149" hidden="1" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="256" hidden="1" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="88" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="150" hidden="1" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="255" hidden="1" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="89" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="151" hidden="1" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="254" hidden="1" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="90" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="152" hidden="1" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="253" hidden="1" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="91" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="153" hidden="1" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="252" hidden="1" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="92" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="154" hidden="1" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="251" hidden="1" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="93" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="119" hidden="1" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="286" hidden="1" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="621" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="155" hidden="1" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="250" hidden="1" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="94" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="156" hidden="1" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="249" hidden="1" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="95" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="157" hidden="1" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="248" hidden="1" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="96" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="158" hidden="1" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="247" hidden="1" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="97" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="159" hidden="1" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="246" hidden="1" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="98" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="160" hidden="1" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="245" hidden="1" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="99" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="161" hidden="1" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="244" hidden="1" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="100" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="162" hidden="1" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="243" hidden="1" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="101" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="163" hidden="1" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="242" hidden="1" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="102" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="164" hidden="1" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="241" hidden="1" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="103" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="120" hidden="1" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="285" hidden="1" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="620" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="165" hidden="1" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="240" hidden="1" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="104" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="166" hidden="1" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="239" hidden="1" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="105" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="167" hidden="1" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="238" hidden="1" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="106" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="168" hidden="1" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="237" hidden="1" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="107" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="169" hidden="1" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="236" hidden="1" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="108" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="170" hidden="1" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="235" hidden="1" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="109" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="171" hidden="1" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="234" hidden="1" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="110" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="172" hidden="1" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="233" hidden="1" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="111" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="173" hidden="1" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="289" hidden="1" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="624" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="174" hidden="1" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="232" hidden="1" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="112" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="121" hidden="1" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="284" hidden="1" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="619" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="175" hidden="1" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="290" hidden="1" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="625" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="176" hidden="1" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="291" hidden="1" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="626" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="177" hidden="1" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="292" hidden="1" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="627" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="178" hidden="1" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="293" hidden="1" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="628" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="179" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="294" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="629" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="180" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="295" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="630" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="181" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="296" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="631" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="182" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="297" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="632" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="183" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="298" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="633" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="184" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="299" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="634" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="122" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="283" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="618" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="185" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="300" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="635" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="186" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="301" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="636" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="187" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="302" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="637" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="188" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="303" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="638" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="189" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="304" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="639" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="190" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="305" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="640" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="191" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="306" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="641" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="192" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="307" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="642" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="193" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="308" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="643" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="194" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="309" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="644" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="123" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="282" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="195" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="310" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="645" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="196" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="311" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="646" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="197" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="312" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="647" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="198" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="313" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="648" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="199" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="314" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="649" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="200" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="315" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="650" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="201" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="316" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="651" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="202" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="317" hidden="1" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="652" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="203" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="318" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="653" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="204" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="319" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="654" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="124" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="281" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="616" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="205" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="320" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="655" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="206" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="321" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="656" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="207" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="322" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="657" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="208" hidden="1" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="323" hidden="1" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="658" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="209" hidden="1" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="324" hidden="1" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="659" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="210" hidden="1" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="325" hidden="1" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="660" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="211" hidden="1" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="326" hidden="1" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="661" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="212" hidden="1" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="327" hidden="1" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="662" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="213" hidden="1" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="328" hidden="1" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="663" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="214" hidden="1" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="329" hidden="1" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="664" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
     <cellStyle name="Input" xfId="23" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input [yellow]" xfId="481"/>
-    <cellStyle name="Input [yellow] 2" xfId="482"/>
-    <cellStyle name="Input [yellow] 2 2" xfId="688"/>
-    <cellStyle name="Input [yellow] 3" xfId="483"/>
-    <cellStyle name="Input [yellow] 3 2" xfId="689"/>
-    <cellStyle name="Input [yellow] 4" xfId="687"/>
-    <cellStyle name="Input 2" xfId="63"/>
-    <cellStyle name="Input 3" xfId="574"/>
-    <cellStyle name="ITEMS" xfId="484"/>
+    <cellStyle name="Input [yellow]" xfId="481" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Input [yellow] 2" xfId="482" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Input [yellow] 2 2" xfId="688" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Input [yellow] 3" xfId="483" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Input [yellow] 3 2" xfId="689" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Input [yellow] 4" xfId="687" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Input 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Input 3" xfId="574" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="ITEMS" xfId="484" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
     <cellStyle name="Linked Cell" xfId="26" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Linked Cell 2" xfId="357"/>
-    <cellStyle name="m1 - Style1" xfId="485"/>
-    <cellStyle name="MANKAD" xfId="486"/>
+    <cellStyle name="Linked Cell 2" xfId="357" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="m1 - Style1" xfId="485" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="MANKAD" xfId="486" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
     <cellStyle name="Neutral" xfId="22" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="354"/>
-    <cellStyle name="Neutrale" xfId="487"/>
-    <cellStyle name="no dec" xfId="488"/>
+    <cellStyle name="Neutral 2" xfId="354" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Neutrale" xfId="487" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="no dec" xfId="488" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="489"/>
-    <cellStyle name="Normal 10" xfId="490"/>
-    <cellStyle name="Normal 11" xfId="419"/>
-    <cellStyle name="Normal 12" xfId="566"/>
-    <cellStyle name="Normal 13" xfId="572"/>
-    <cellStyle name="Normal 14" xfId="577"/>
-    <cellStyle name="Normal 14 2" xfId="580"/>
-    <cellStyle name="Normal 14 3" xfId="593"/>
-    <cellStyle name="Normal 14 3 2" xfId="600"/>
-    <cellStyle name="Normal 14 3 2 2" xfId="604"/>
-    <cellStyle name="Normal 14 3 2 2 2" xfId="607"/>
-    <cellStyle name="Normal 14 4" xfId="595"/>
-    <cellStyle name="Normal 14 4 2" xfId="597"/>
-    <cellStyle name="Normal 14 4 2 2" xfId="601"/>
-    <cellStyle name="Normal 14 4 2 2 2" xfId="605"/>
-    <cellStyle name="Normal 15" xfId="588"/>
-    <cellStyle name="Normal 16" xfId="609"/>
-    <cellStyle name="Normal 17" xfId="610"/>
-    <cellStyle name="Normal 18" xfId="60"/>
-    <cellStyle name="Normal 19" xfId="576"/>
-    <cellStyle name="Normal 2" xfId="66"/>
-    <cellStyle name="Normal 2 2" xfId="231"/>
-    <cellStyle name="Normal 2 2 2" xfId="346"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="492"/>
-    <cellStyle name="Normal 2 2 3" xfId="493"/>
-    <cellStyle name="Normal 2 2 4" xfId="491"/>
-    <cellStyle name="Normal 2 3" xfId="494"/>
-    <cellStyle name="Normal 3" xfId="229"/>
-    <cellStyle name="Normal 3 2" xfId="345"/>
-    <cellStyle name="Normal 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 3 3" xfId="497"/>
-    <cellStyle name="Normal 3 4" xfId="495"/>
-    <cellStyle name="Normal 4" xfId="383"/>
-    <cellStyle name="Normal 4 2" xfId="499"/>
-    <cellStyle name="Normal 4 3" xfId="498"/>
-    <cellStyle name="Normal 5" xfId="387"/>
-    <cellStyle name="Normal 5 2" xfId="500"/>
-    <cellStyle name="Normal 6" xfId="401"/>
-    <cellStyle name="Normal 6 2" xfId="501"/>
-    <cellStyle name="Normal 7" xfId="415"/>
-    <cellStyle name="Normal 7 2" xfId="417"/>
-    <cellStyle name="Normal 7 3" xfId="502"/>
-    <cellStyle name="Normal 7 3 2" xfId="564"/>
-    <cellStyle name="Normal 7 3 2 2" xfId="570"/>
-    <cellStyle name="Normal 8" xfId="503"/>
-    <cellStyle name="Normal 8 2" xfId="504"/>
-    <cellStyle name="Normal 8 2 2" xfId="560"/>
-    <cellStyle name="Normal 8 3" xfId="561"/>
-    <cellStyle name="Normal 8 3 2" xfId="591"/>
-    <cellStyle name="Normal 8 3 2 2" xfId="608"/>
-    <cellStyle name="Normal 9" xfId="505"/>
-    <cellStyle name="Normal 9 2" xfId="558"/>
-    <cellStyle name="Normal 9 3" xfId="565"/>
-    <cellStyle name="Normal 9 4" xfId="568"/>
-    <cellStyle name="Normal 9 5" xfId="569"/>
-    <cellStyle name="Normal 9 6" xfId="571"/>
-    <cellStyle name="Normal 9 6 2" xfId="592"/>
-    <cellStyle name="Normal 9 6 2 2" xfId="611"/>
-    <cellStyle name="Nota" xfId="506"/>
-    <cellStyle name="Nota 2" xfId="507"/>
-    <cellStyle name="Nota 2 2" xfId="691"/>
-    <cellStyle name="Nota 3" xfId="508"/>
-    <cellStyle name="Nota 3 2" xfId="692"/>
-    <cellStyle name="Nota 4" xfId="690"/>
+    <cellStyle name="Normal - Style1" xfId="489" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 10" xfId="490" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 11" xfId="419" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 12" xfId="566" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 13" xfId="572" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 14" xfId="577" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 14 2" xfId="580" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 14 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 14 3 2" xfId="600" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 14 3 2 2" xfId="604" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 14 3 2 2 2" xfId="607" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 14 4" xfId="595" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 14 4 2" xfId="597" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 14 4 2 2" xfId="601" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 14 4 2 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 15" xfId="588" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 16" xfId="609" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 17" xfId="610" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 18" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 19" xfId="576" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 2" xfId="66" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 2 2" xfId="231" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="346" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="492" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="493" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="491" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 2 3" xfId="494" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 3" xfId="229" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 3 2" xfId="345" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 3 3" xfId="497" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 4" xfId="383" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 4 2" xfId="499" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 4 3" xfId="498" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 5" xfId="387" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 5 2" xfId="500" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6" xfId="401" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 2" xfId="501" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 7" xfId="415" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 7 2" xfId="417" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 7 3" xfId="502" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 7 3 2" xfId="564" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 7 3 2 2" xfId="570" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 8" xfId="503" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 8 2" xfId="504" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 8 3" xfId="561" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 8 3 2" xfId="591" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 8 3 2 2" xfId="608" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 9" xfId="505" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 9 2" xfId="558" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 9 3" xfId="565" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 9 4" xfId="568" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 9 5" xfId="569" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 9 6" xfId="571" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 9 6 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 9 6 2 2" xfId="611" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Nota" xfId="506" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Nota 2" xfId="507" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Nota 2 2" xfId="691" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Nota 3" xfId="508" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Nota 3 2" xfId="692" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Nota 4" xfId="690" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
     <cellStyle name="Note" xfId="29" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="384"/>
-    <cellStyle name="Note 3" xfId="388"/>
-    <cellStyle name="Note 4" xfId="402"/>
-    <cellStyle name="Num0 - Style7" xfId="509"/>
-    <cellStyle name="Num2 - Style8" xfId="510"/>
-    <cellStyle name="Numeri - Style1" xfId="511"/>
-    <cellStyle name="Numeri - Style1 2" xfId="512"/>
-    <cellStyle name="Numeri - Style1 2 2" xfId="694"/>
-    <cellStyle name="Numeri - Style1 3" xfId="693"/>
-    <cellStyle name="ofwhich" xfId="64"/>
+    <cellStyle name="Note 2" xfId="384" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Note 3" xfId="388" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Note 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Num0 - Style7" xfId="509" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Num2 - Style8" xfId="510" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Numeri - Style1" xfId="511" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Numeri - Style1 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Numeri - Style1 2 2" xfId="694" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Numeri - Style1 3" xfId="693" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="ofwhich" xfId="64" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
     <cellStyle name="Output" xfId="24" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="355"/>
-    <cellStyle name="Parent row" xfId="5"/>
-    <cellStyle name="Percent [2]" xfId="513"/>
-    <cellStyle name="Percent 10" xfId="575"/>
-    <cellStyle name="Percent 2" xfId="67"/>
-    <cellStyle name="Percent 2 2" xfId="423"/>
-    <cellStyle name="Percent 3" xfId="514"/>
-    <cellStyle name="Percent 3 2" xfId="515"/>
-    <cellStyle name="Percent 3 3" xfId="516"/>
-    <cellStyle name="Percent 3 4" xfId="563"/>
-    <cellStyle name="Percent 4" xfId="517"/>
-    <cellStyle name="Percent 4 2" xfId="518"/>
-    <cellStyle name="Percent 5" xfId="519"/>
-    <cellStyle name="Percent 6" xfId="421"/>
-    <cellStyle name="Percent 7" xfId="567"/>
-    <cellStyle name="Percent 8" xfId="585"/>
-    <cellStyle name="Percent 8 2" xfId="594"/>
-    <cellStyle name="Percent 8 3" xfId="596"/>
-    <cellStyle name="Percent 8 3 2" xfId="599"/>
-    <cellStyle name="Percent 8 3 2 2" xfId="603"/>
-    <cellStyle name="Percent 8 3 2 2 2" xfId="606"/>
-    <cellStyle name="Percent 9" xfId="61"/>
-    <cellStyle name="RevList" xfId="520"/>
-    <cellStyle name="Row headings" xfId="521"/>
-    <cellStyle name="Row headings Level 1" xfId="522"/>
-    <cellStyle name="Row headings Level 2" xfId="523"/>
-    <cellStyle name="Section Break" xfId="7"/>
-    <cellStyle name="Section Break: parent row" xfId="4"/>
-    <cellStyle name="Source - Style2" xfId="524"/>
-    <cellStyle name="Sources list" xfId="525"/>
-    <cellStyle name="Sources list 2" xfId="526"/>
-    <cellStyle name="Sources Title" xfId="527"/>
-    <cellStyle name="Sources Title 2" xfId="528"/>
-    <cellStyle name="style" xfId="529"/>
-    <cellStyle name="style 2" xfId="530"/>
-    <cellStyle name="style 2 2" xfId="696"/>
-    <cellStyle name="style 3" xfId="531"/>
-    <cellStyle name="style 3 2" xfId="697"/>
-    <cellStyle name="style 4" xfId="695"/>
-    <cellStyle name="style1" xfId="532"/>
-    <cellStyle name="style2" xfId="533"/>
-    <cellStyle name="Subtotal" xfId="534"/>
-    <cellStyle name="Table  - Style3" xfId="535"/>
-    <cellStyle name="Table  - Style4" xfId="536"/>
-    <cellStyle name="Table  - Style4 2" xfId="537"/>
-    <cellStyle name="Table  - Style6" xfId="538"/>
-    <cellStyle name="Table  - Style6 2" xfId="539"/>
-    <cellStyle name="Table no" xfId="540"/>
-    <cellStyle name="Table title" xfId="12"/>
-    <cellStyle name="Table_HeaderRow" xfId="65"/>
-    <cellStyle name="Testo avviso" xfId="541"/>
-    <cellStyle name="Testo descrittivo" xfId="542"/>
-    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="543"/>
-    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="544"/>
+    <cellStyle name="Output 2" xfId="355" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Percent [2]" xfId="513" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Percent 10" xfId="575" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Percent 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Percent 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Percent 3" xfId="514" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Percent 3 2" xfId="515" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Percent 3 3" xfId="516" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Percent 3 4" xfId="563" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Percent 4" xfId="517" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Percent 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Percent 5" xfId="519" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Percent 6" xfId="421" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Percent 7" xfId="567" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Percent 8" xfId="585" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Percent 8 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Percent 8 3" xfId="596" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Percent 8 3 2" xfId="599" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Percent 8 3 2 2" xfId="603" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Percent 8 3 2 2 2" xfId="606" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Percent 9" xfId="61" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="RevList" xfId="520" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Row headings" xfId="521" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Row headings Level 1" xfId="522" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Row headings Level 2" xfId="523" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Section Break" xfId="7" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Section Break: parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Source - Style2" xfId="524" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Sources list" xfId="525" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Sources list 2" xfId="526" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Sources Title" xfId="527" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Sources Title 2" xfId="528" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="style" xfId="529" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="style 2" xfId="530" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
+    <cellStyle name="style 2 2" xfId="696" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
+    <cellStyle name="style 3" xfId="531" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
+    <cellStyle name="style 3 2" xfId="697" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
+    <cellStyle name="style 4" xfId="695" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
+    <cellStyle name="style1" xfId="532" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
+    <cellStyle name="style2" xfId="533" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
+    <cellStyle name="Subtotal" xfId="534" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
+    <cellStyle name="Table  - Style3" xfId="535" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
+    <cellStyle name="Table  - Style4" xfId="536" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
+    <cellStyle name="Table  - Style4 2" xfId="537" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
+    <cellStyle name="Table  - Style6" xfId="538" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
+    <cellStyle name="Table  - Style6 2" xfId="539" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
+    <cellStyle name="Table no" xfId="540" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
+    <cellStyle name="Table title" xfId="12" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
+    <cellStyle name="Table_HeaderRow" xfId="65" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
+    <cellStyle name="Testo avviso" xfId="541" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
+    <cellStyle name="Testo descrittivo" xfId="542" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
+    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="543" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
+    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="544" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
     <cellStyle name="Title" xfId="15" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title-2" xfId="56"/>
-    <cellStyle name="Titolo" xfId="545"/>
-    <cellStyle name="Titolo 1" xfId="546"/>
-    <cellStyle name="Titolo 2" xfId="547"/>
-    <cellStyle name="Titolo 3" xfId="548"/>
-    <cellStyle name="Titolo 4" xfId="549"/>
+    <cellStyle name="Title-2" xfId="56" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
+    <cellStyle name="Titolo" xfId="545" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
+    <cellStyle name="Titolo 1" xfId="546" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
+    <cellStyle name="Titolo 2" xfId="547" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
+    <cellStyle name="Titolo 3" xfId="548" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
+    <cellStyle name="Titolo 4" xfId="549" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
     <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="361"/>
-    <cellStyle name="Totale" xfId="550"/>
-    <cellStyle name="Totale 2" xfId="551"/>
-    <cellStyle name="Totale 2 2" xfId="699"/>
-    <cellStyle name="Totale 3" xfId="552"/>
-    <cellStyle name="Totale 3 2" xfId="700"/>
-    <cellStyle name="Totale 4" xfId="698"/>
-    <cellStyle name="Valore non valido" xfId="553"/>
-    <cellStyle name="Valore valido" xfId="554"/>
+    <cellStyle name="Total 2" xfId="361" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
+    <cellStyle name="Totale" xfId="550" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
+    <cellStyle name="Totale 2" xfId="551" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
+    <cellStyle name="Totale 2 2" xfId="699" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
+    <cellStyle name="Totale 3" xfId="552" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
+    <cellStyle name="Totale 3 2" xfId="700" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
+    <cellStyle name="Totale 4" xfId="698" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
+    <cellStyle name="Valore non valido" xfId="553" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
+    <cellStyle name="Valore valido" xfId="554" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
     <cellStyle name="Warning Text" xfId="28" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Warning Text 2" xfId="359"/>
+    <cellStyle name="Warning Text 2" xfId="359" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -3553,17 +3561,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
-    <tableStyle name="EnergyCalcTables" pivot="0" count="4">
+    <tableStyle name="EnergyCalcTables" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0"/>
+    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3652,6 +3660,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3687,6 +3712,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3862,16 +3904,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="132.265625" customWidth="1"/>
+    <col min="2" max="2" width="132.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3941,6 +3983,11 @@
     <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3950,21 +3997,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1328125" customWidth="1"/>
-    <col min="15" max="15" width="14.73046875" customWidth="1"/>
-    <col min="16" max="16" width="19.73046875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1">
@@ -3984,10 +4031,10 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>60</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -3997,533 +4044,533 @@
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>7.3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="J3" s="40" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="16"/>
+      <c r="J3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="37"/>
+      <c r="K3" s="36"/>
       <c r="M3" s="3">
         <v>5.3</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="23"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="17"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="16"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="38"/>
+      <c r="K4" s="37"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="23"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="40">
         <f>AVERAGE(G12:G17)</f>
         <v>18.333333333333332</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="37"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="23"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="25">
+      <c r="F6" s="20"/>
+      <c r="G6" s="24">
         <v>10</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="37"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="O6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="Q6" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="21" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="25">
+      <c r="F7" s="20"/>
+      <c r="G7" s="24">
         <v>10</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="40">
         <f>AVERAGE(G27:G30)</f>
         <v>9</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="37"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29" t="s">
+      <c r="N7" s="27"/>
+      <c r="O7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="Q7" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="23"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="21" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="25">
+      <c r="F8" s="20"/>
+      <c r="G8" s="24">
         <v>10</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="37"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="28" t="s">
+      <c r="N8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29" t="s">
+      <c r="O8" s="28"/>
+      <c r="P8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q8" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="21" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="25">
+      <c r="F9" s="20"/>
+      <c r="G9" s="24">
         <v>10</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="41">
         <f>(J5*G41+J7*G44)/SUM(G41,G44)</f>
         <v>16.402434831574382</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="37">
         <f>Q7</f>
         <v>10</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29" t="s">
+      <c r="N9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="Q9" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="16" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="25">
+      <c r="F10" s="20"/>
+      <c r="G10" s="24">
         <v>10</v>
       </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33" t="s">
+      <c r="O10" s="32"/>
+      <c r="P10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="34">
+      <c r="Q10" s="33">
         <v>31.877221924034789</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="21" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="25">
+      <c r="F11" s="20"/>
+      <c r="G11" s="24">
         <v>10</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="16" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="25">
+      <c r="F12" s="20"/>
+      <c r="G12" s="24">
         <v>20</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="37"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="23"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="21" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25">
+      <c r="F13" s="20"/>
+      <c r="G13" s="24">
         <v>20</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="40">
         <v>10</v>
       </c>
-      <c r="K13" s="38"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="23"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="21" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="25">
+      <c r="F14" s="20"/>
+      <c r="G14" s="24">
         <v>20</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="38"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="23"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="21" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="25">
+      <c r="F15" s="20"/>
+      <c r="G15" s="24">
         <v>20</v>
       </c>
-      <c r="J15" s="41">
+      <c r="J15" s="40">
         <v>10</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="37"/>
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="23"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="21" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="25">
+      <c r="F16" s="20"/>
+      <c r="G16" s="24">
         <v>15</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="37"/>
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="21" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="25">
+      <c r="F17" s="20"/>
+      <c r="G17" s="24">
         <v>15</v>
       </c>
-      <c r="J17" s="42">
+      <c r="J17" s="41">
         <f>AVERAGE(J13:J15)</f>
         <v>10</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="37">
         <f>Q6</f>
         <v>10</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="23"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="16" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="25">
+      <c r="F18" s="20"/>
+      <c r="G18" s="24">
         <v>12</v>
       </c>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="23"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="21" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="25">
+      <c r="F19" s="20"/>
+      <c r="G19" s="24">
         <v>12</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="43"/>
+      <c r="K19" s="42"/>
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="23"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="21" t="s">
+      <c r="A20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="25">
+      <c r="F20" s="20"/>
+      <c r="G20" s="24">
         <v>12</v>
       </c>
-      <c r="J20" s="38" t="s">
+      <c r="J20" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="38"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="23"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="21" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="25">
+      <c r="F21" s="20"/>
+      <c r="G21" s="24">
         <v>12</v>
       </c>
-      <c r="J21" s="38">
+      <c r="J21" s="37">
         <v>20</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="43">
         <f>Q10</f>
         <v>31.877221924034789</v>
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="23"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="16" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="25">
+      <c r="F22" s="20"/>
+      <c r="G22" s="24">
         <v>8</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="23"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="21" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="25">
+      <c r="F23" s="20"/>
+      <c r="G23" s="24">
         <v>8</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="43"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="23"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="21" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="25">
+      <c r="F24" s="20"/>
+      <c r="G24" s="24">
         <v>8</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J24" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="38"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="23"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="21" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="25">
+      <c r="F25" s="20"/>
+      <c r="G25" s="24">
         <v>8</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J25" s="37">
         <v>35</v>
       </c>
-      <c r="K25" s="38">
+      <c r="K25" s="37">
         <f>Q9</f>
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="23"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="21" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="25">
+      <c r="F26" s="20"/>
+      <c r="G26" s="24">
         <v>5</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="23"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="16" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="25">
+      <c r="F27" s="20"/>
+      <c r="G27" s="24">
         <v>8</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -4532,15 +4579,15 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="23"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="21" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="26">
+      <c r="F28" s="20"/>
+      <c r="G28" s="25">
         <v>8</v>
       </c>
       <c r="J28" t="s">
@@ -4548,32 +4595,32 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="23"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="21" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="26">
+      <c r="F29" s="20"/>
+      <c r="G29" s="25">
         <v>8</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <f>AVERAGE(G18:G21)</f>
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="23"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="21" t="s">
+      <c r="A30" s="22"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="26">
+      <c r="F30" s="20"/>
+      <c r="G30" s="25">
         <v>12</v>
       </c>
       <c r="J30" t="s">
@@ -4581,36 +4628,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="23"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="15" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="27">
+      <c r="F31" s="20"/>
+      <c r="G31" s="26">
         <v>35</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="10">
         <f>AVERAGE(G22:G26)</f>
         <v>7.4</v>
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="23"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="21" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="27">
+      <c r="F32" s="20"/>
+      <c r="G32" s="26">
         <v>35</v>
       </c>
       <c r="J32" t="s">
@@ -4618,28 +4665,28 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="23"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="13" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="24">
+      <c r="F33" s="13"/>
+      <c r="G33" s="23">
         <v>20</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="9">
         <f>AVERAGE(J29:J31)</f>
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15">
-      <c r="B36" s="45" t="s">
+    <row r="36" spans="1:14" ht="15.75">
+      <c r="B36" s="44" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4927,25 +4974,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:3" ht="45">
+      <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -4960,8 +5007,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="8">
-        <f>('India Data'!J9)</f>
-        <v>16.402434831574382</v>
+        <f>'India Data'!J5</f>
+        <v>18.333333333333332</v>
       </c>
       <c r="C2">
         <f>'India Data'!K9</f>
@@ -5011,11 +5058,11 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <f>B6</f>
+      <c r="B6" s="46">
+        <f>'India Data'!J7</f>
+        <v>9</v>
+      </c>
+      <c r="C6" s="45">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corresponding edits to High GDP files
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\trans\AVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683937AB-F5C5-49F8-95B7-31920D8FD88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="10" yWindow="260" windowWidth="19190" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="India Data" sheetId="12" r:id="rId2"/>
     <sheet name="AVL" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
   <si>
     <t>ships</t>
   </si>
@@ -227,12 +231,15 @@
   </si>
   <si>
     <t>Public Private share of Passenger Km in Road Transport</t>
+  </si>
+  <si>
+    <t>For India, passenger ships are repurposed as taxis.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="17">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2692,7 +2699,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2706,7 +2713,6 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="33" fillId="36" borderId="21" xfId="576" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2777,710 +2783,712 @@
     <xf numFmtId="0" fontId="102" fillId="65" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="702">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="227"/>
-    <cellStyle name="20% - Accent1 3" xfId="385"/>
-    <cellStyle name="20% - Accent1 4" xfId="389"/>
-    <cellStyle name="20% - Accent1 5" xfId="403"/>
+    <cellStyle name="20% - Accent1 2" xfId="227" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="385" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent1 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent1 5" xfId="403" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="20% - Accent2" xfId="37" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="391"/>
-    <cellStyle name="20% - Accent2 3" xfId="405"/>
-    <cellStyle name="20% - Accent2 4" xfId="366"/>
+    <cellStyle name="20% - Accent2 2" xfId="391" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Accent2 3" xfId="405" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent2 4" xfId="366" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="20% - Accent3" xfId="41" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="393"/>
-    <cellStyle name="20% - Accent3 3" xfId="407"/>
-    <cellStyle name="20% - Accent3 4" xfId="370"/>
+    <cellStyle name="20% - Accent3 2" xfId="393" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent3 3" xfId="407" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - Accent3 4" xfId="370" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="20% - Accent4" xfId="45" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="395"/>
-    <cellStyle name="20% - Accent4 3" xfId="409"/>
-    <cellStyle name="20% - Accent4 4" xfId="374"/>
+    <cellStyle name="20% - Accent4 2" xfId="395" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - Accent4 3" xfId="409" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - Accent4 4" xfId="374" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="20% - Accent5" xfId="49" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="397"/>
-    <cellStyle name="20% - Accent5 3" xfId="411"/>
-    <cellStyle name="20% - Accent5 4" xfId="378"/>
+    <cellStyle name="20% - Accent5 2" xfId="397" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - Accent5 3" xfId="411" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - Accent5 4" xfId="378" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="20% - Accent6" xfId="53" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 10" xfId="590"/>
-    <cellStyle name="20% - Accent6 2" xfId="117"/>
-    <cellStyle name="20% - Accent6 3" xfId="344"/>
-    <cellStyle name="20% - Accent6 3 2" xfId="556"/>
-    <cellStyle name="20% - Accent6 4" xfId="347"/>
-    <cellStyle name="20% - Accent6 4 2" xfId="418"/>
-    <cellStyle name="20% - Accent6 5" xfId="386"/>
-    <cellStyle name="20% - Accent6 6" xfId="399"/>
-    <cellStyle name="20% - Accent6 7" xfId="413"/>
-    <cellStyle name="20% - Accent6 8" xfId="559"/>
-    <cellStyle name="20% - Accent6 9" xfId="578"/>
-    <cellStyle name="20% - Colore 1" xfId="424"/>
-    <cellStyle name="20% - Colore 2" xfId="425"/>
-    <cellStyle name="20% - Colore 3" xfId="426"/>
-    <cellStyle name="20% - Colore 4" xfId="427"/>
-    <cellStyle name="20% - Colore 5" xfId="428"/>
-    <cellStyle name="20% - Colore 6" xfId="429"/>
+    <cellStyle name="20% - Accent6 10" xfId="590" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - Accent6 3" xfId="344" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="20% - Accent6 3 2" xfId="556" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="20% - Accent6 4" xfId="347" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="20% - Accent6 4 2" xfId="418" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - Accent6 5" xfId="386" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="20% - Accent6 6" xfId="399" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Accent6 7" xfId="413" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="20% - Accent6 8" xfId="559" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="20% - Accent6 9" xfId="578" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="20% - Colore 1" xfId="424" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="20% - Colore 2" xfId="425" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="20% - Colore 3" xfId="426" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - Colore 4" xfId="427" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="20% - Colore 5" xfId="428" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - Colore 6" xfId="429" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="40% - Accent1" xfId="34" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="390"/>
-    <cellStyle name="40% - Accent1 3" xfId="404"/>
-    <cellStyle name="40% - Accent1 4" xfId="363"/>
+    <cellStyle name="40% - Accent1 2" xfId="390" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="40% - Accent1 3" xfId="404" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="40% - Accent1 4" xfId="363" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="40% - Accent2" xfId="38" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="392"/>
-    <cellStyle name="40% - Accent2 3" xfId="406"/>
-    <cellStyle name="40% - Accent2 4" xfId="367"/>
+    <cellStyle name="40% - Accent2 2" xfId="392" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="40% - Accent2 3" xfId="406" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="40% - Accent2 4" xfId="367" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="40% - Accent3" xfId="42" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="394"/>
-    <cellStyle name="40% - Accent3 3" xfId="408"/>
-    <cellStyle name="40% - Accent3 4" xfId="371"/>
+    <cellStyle name="40% - Accent3 2" xfId="394" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="40% - Accent3 3" xfId="408" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="40% - Accent3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="40% - Accent4" xfId="46" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="396"/>
-    <cellStyle name="40% - Accent4 3" xfId="410"/>
-    <cellStyle name="40% - Accent4 4" xfId="375"/>
+    <cellStyle name="40% - Accent4 2" xfId="396" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="40% - Accent4 3" xfId="410" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="40% - Accent4 4" xfId="375" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="40% - Accent5" xfId="50" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="398"/>
-    <cellStyle name="40% - Accent5 3" xfId="412"/>
-    <cellStyle name="40% - Accent5 4" xfId="379"/>
+    <cellStyle name="40% - Accent5 2" xfId="398" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="40% - Accent5 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="40% - Accent5 4" xfId="379" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
     <cellStyle name="40% - Accent6" xfId="54" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="400"/>
-    <cellStyle name="40% - Accent6 3" xfId="414"/>
-    <cellStyle name="40% - Accent6 4" xfId="381"/>
-    <cellStyle name="40% - Colore 1" xfId="430"/>
-    <cellStyle name="40% - Colore 2" xfId="431"/>
-    <cellStyle name="40% - Colore 3" xfId="432"/>
-    <cellStyle name="40% - Colore 4" xfId="433"/>
-    <cellStyle name="40% - Colore 5" xfId="434"/>
-    <cellStyle name="40% - Colore 6" xfId="435"/>
+    <cellStyle name="40% - Accent6 2" xfId="400" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="40% - Accent6 3" xfId="414" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="40% - Accent6 4" xfId="381" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="40% - Colore 1" xfId="430" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="40% - Colore 2" xfId="431" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="40% - Colore 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="40% - Colore 4" xfId="433" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="40% - Colore 5" xfId="434" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="40% - Colore 6" xfId="435" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
     <cellStyle name="60% - Accent1" xfId="35" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1 2" xfId="364"/>
+    <cellStyle name="60% - Accent1 2" xfId="364" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
     <cellStyle name="60% - Accent2" xfId="39" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2 2" xfId="368"/>
+    <cellStyle name="60% - Accent2 2" xfId="368" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="60% - Accent3" xfId="43" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3 2" xfId="372"/>
+    <cellStyle name="60% - Accent3 2" xfId="372" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
     <cellStyle name="60% - Accent4" xfId="47" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4 2" xfId="376"/>
+    <cellStyle name="60% - Accent4 2" xfId="376" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
     <cellStyle name="60% - Accent5" xfId="51" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5 2" xfId="380"/>
+    <cellStyle name="60% - Accent5 2" xfId="380" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
     <cellStyle name="60% - Accent6" xfId="55" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6 2" xfId="382"/>
-    <cellStyle name="60% - Colore 1" xfId="436"/>
-    <cellStyle name="60% - Colore 2" xfId="437"/>
-    <cellStyle name="60% - Colore 3" xfId="438"/>
-    <cellStyle name="60% - Colore 4" xfId="439"/>
-    <cellStyle name="60% - Colore 5" xfId="440"/>
-    <cellStyle name="60% - Colore 6" xfId="441"/>
-    <cellStyle name="A - a heading" xfId="581"/>
-    <cellStyle name="A - bold" xfId="584"/>
-    <cellStyle name="A - bottom border" xfId="586"/>
-    <cellStyle name="A - bottom border 2" xfId="701"/>
-    <cellStyle name="A - header" xfId="583"/>
-    <cellStyle name="A - header 2" xfId="598"/>
-    <cellStyle name="A - header 2 2" xfId="602"/>
-    <cellStyle name="A - normal" xfId="582"/>
-    <cellStyle name="A - percent" xfId="587"/>
+    <cellStyle name="60% - Accent6 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="60% - Colore 1" xfId="436" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="60% - Colore 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="60% - Colore 3" xfId="438" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="60% - Colore 4" xfId="439" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="60% - Colore 5" xfId="440" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="60% - Colore 6" xfId="441" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="A - a heading" xfId="581" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="A - bold" xfId="584" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="A - bottom border" xfId="586" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="A - bottom border 2" xfId="701" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="A - header" xfId="583" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="A - header 2" xfId="598" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="A - header 2 2" xfId="602" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="A - normal" xfId="582" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="A - percent" xfId="587" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
     <cellStyle name="Accent1" xfId="32" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 2" xfId="362"/>
+    <cellStyle name="Accent1 2" xfId="362" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
     <cellStyle name="Accent2" xfId="36" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="365"/>
+    <cellStyle name="Accent2 2" xfId="365" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
     <cellStyle name="Accent3" xfId="40" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="369"/>
+    <cellStyle name="Accent3 2" xfId="369" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
     <cellStyle name="Accent4" xfId="44" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="373"/>
+    <cellStyle name="Accent4 2" xfId="373" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
     <cellStyle name="Accent5" xfId="48" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="377"/>
+    <cellStyle name="Accent5 2" xfId="377" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
     <cellStyle name="Accent6" xfId="52" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="348"/>
+    <cellStyle name="Accent6 2" xfId="348" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
     <cellStyle name="Bad" xfId="21" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="353"/>
-    <cellStyle name="Best" xfId="442"/>
-    <cellStyle name="Body: normal cell" xfId="2"/>
-    <cellStyle name="BORDERS" xfId="443"/>
-    <cellStyle name="BORDERS 2" xfId="444"/>
-    <cellStyle name="BORDERS 2 2" xfId="679"/>
-    <cellStyle name="BORDERS 3" xfId="678"/>
-    <cellStyle name="Calc Currency (0)" xfId="445"/>
-    <cellStyle name="Calcolo" xfId="446"/>
-    <cellStyle name="Calcolo 2" xfId="447"/>
-    <cellStyle name="Calcolo 2 2" xfId="681"/>
-    <cellStyle name="Calcolo 3" xfId="448"/>
-    <cellStyle name="Calcolo 3 2" xfId="682"/>
-    <cellStyle name="Calcolo 4" xfId="680"/>
+    <cellStyle name="Bad 2" xfId="353" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Best" xfId="442" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="BORDERS" xfId="443" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="BORDERS 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="BORDERS 2 2" xfId="679" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="BORDERS 3" xfId="678" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Calc Currency (0)" xfId="445" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Calcolo" xfId="446" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Calcolo 2" xfId="447" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Calcolo 2 2" xfId="681" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Calcolo 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Calcolo 3 2" xfId="682" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Calcolo 4" xfId="680" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
     <cellStyle name="Calculation" xfId="25" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Calculation 2" xfId="356"/>
-    <cellStyle name="Cella collegata" xfId="449"/>
-    <cellStyle name="Cella da controllare" xfId="450"/>
+    <cellStyle name="Calculation 2" xfId="356" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Cella collegata" xfId="449" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Cella da controllare" xfId="450" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Check Cell 2" xfId="358"/>
-    <cellStyle name="Colore 1" xfId="451"/>
-    <cellStyle name="Colore 2" xfId="452"/>
-    <cellStyle name="Colore 3" xfId="453"/>
-    <cellStyle name="Colore 4" xfId="454"/>
-    <cellStyle name="Colore 5" xfId="455"/>
-    <cellStyle name="Colore 6" xfId="456"/>
-    <cellStyle name="Column - Style5" xfId="457"/>
-    <cellStyle name="Column - Style6" xfId="458"/>
-    <cellStyle name="Column headings" xfId="459"/>
-    <cellStyle name="Column headings 2" xfId="683"/>
-    <cellStyle name="Comma 2" xfId="230"/>
-    <cellStyle name="Comma 2 2" xfId="460"/>
-    <cellStyle name="Comma 2 3" xfId="420"/>
-    <cellStyle name="Comma 2 4" xfId="573"/>
-    <cellStyle name="Comma 3" xfId="416"/>
-    <cellStyle name="Comma 3 2" xfId="462"/>
-    <cellStyle name="Comma 3 3" xfId="461"/>
-    <cellStyle name="Comma 4" xfId="463"/>
-    <cellStyle name="Comma 4 2" xfId="562"/>
-    <cellStyle name="Comma 5" xfId="464"/>
-    <cellStyle name="Comma 6" xfId="422"/>
-    <cellStyle name="Comma 7" xfId="579"/>
-    <cellStyle name="Comma 8" xfId="589"/>
-    <cellStyle name="Comma 9" xfId="62"/>
-    <cellStyle name="Comma0" xfId="465"/>
-    <cellStyle name="Copied" xfId="466"/>
-    <cellStyle name="Currency 2" xfId="557"/>
-    <cellStyle name="Currency0" xfId="467"/>
-    <cellStyle name="Data" xfId="13"/>
-    <cellStyle name="Data (Number)" xfId="468"/>
-    <cellStyle name="Data (Text)" xfId="469"/>
-    <cellStyle name="Data no deci" xfId="59"/>
-    <cellStyle name="Date" xfId="470"/>
-    <cellStyle name="Entered" xfId="471"/>
-    <cellStyle name="Excel Built-in Normal" xfId="114"/>
+    <cellStyle name="Check Cell 2" xfId="358" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Colore 1" xfId="451" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Colore 2" xfId="452" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Colore 3" xfId="453" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Colore 4" xfId="454" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Colore 5" xfId="455" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Colore 6" xfId="456" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Column - Style5" xfId="457" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Column - Style6" xfId="458" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Column headings" xfId="459" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Column headings 2" xfId="683" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Comma 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Comma 2 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Comma 2 3" xfId="420" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Comma 2 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Comma 3" xfId="416" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Comma 3 2" xfId="462" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Comma 3 3" xfId="461" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Comma 4" xfId="463" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Comma 4 2" xfId="562" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Comma 5" xfId="464" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Comma 6" xfId="422" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Comma 7" xfId="579" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Comma 8" xfId="589" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Comma 9" xfId="62" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Comma0" xfId="465" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Copied" xfId="466" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Currency 2" xfId="557" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Currency0" xfId="467" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Data" xfId="13" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Data (Number)" xfId="468" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Data (Text)" xfId="469" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Data no deci" xfId="59" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Date" xfId="470" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Entered" xfId="471" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="114" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
     <cellStyle name="Explanatory Text" xfId="30" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="360"/>
-    <cellStyle name="FIGURES" xfId="472"/>
-    <cellStyle name="Fixed" xfId="473"/>
+    <cellStyle name="Explanatory Text 2" xfId="360" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="FIGURES" xfId="472" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Fixed" xfId="473" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="8"/>
-    <cellStyle name="Footnote Text" xfId="474"/>
-    <cellStyle name="Footnotes: all except top row" xfId="11"/>
-    <cellStyle name="Footnotes: top row" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="8" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Footnote Text" xfId="474" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="11" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
     <cellStyle name="Good" xfId="20" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="343"/>
-    <cellStyle name="Grey" xfId="475"/>
-    <cellStyle name="Header: bottom row" xfId="1"/>
-    <cellStyle name="Header: top rows" xfId="3"/>
-    <cellStyle name="Header1" xfId="476"/>
-    <cellStyle name="Header2" xfId="477"/>
-    <cellStyle name="Header2 2" xfId="478"/>
-    <cellStyle name="Header2 2 2" xfId="685"/>
-    <cellStyle name="Header2 3" xfId="479"/>
-    <cellStyle name="Header2 3 2" xfId="686"/>
-    <cellStyle name="Header2 4" xfId="684"/>
+    <cellStyle name="Good 2" xfId="343" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Grey" xfId="475" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Header: bottom row" xfId="1" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Header: top rows" xfId="3" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Header1" xfId="476" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Header2" xfId="477" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Header2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Header2 2 2" xfId="685" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Header2 3" xfId="479" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Header2 3 2" xfId="686" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Header2 4" xfId="684" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
     <cellStyle name="Heading 1" xfId="16" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 1 2" xfId="349"/>
+    <cellStyle name="Heading 1 2" xfId="349" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
     <cellStyle name="Heading 2" xfId="17" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 2 2" xfId="350"/>
+    <cellStyle name="Heading 2 2" xfId="350" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
     <cellStyle name="Heading 3" xfId="18" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 3 2" xfId="351"/>
+    <cellStyle name="Heading 3 2" xfId="351" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
     <cellStyle name="Heading 4" xfId="19" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Heading 4 2" xfId="352"/>
-    <cellStyle name="Hed Side" xfId="14"/>
-    <cellStyle name="Hed Side Regular" xfId="58"/>
-    <cellStyle name="Hed Top" xfId="57"/>
-    <cellStyle name="Hyperlink 10" xfId="125" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="280" hidden="1"/>
-    <cellStyle name="Hyperlink 10" xfId="615"/>
-    <cellStyle name="Hyperlink 100" xfId="215" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="330" hidden="1"/>
-    <cellStyle name="Hyperlink 100" xfId="665"/>
-    <cellStyle name="Hyperlink 101" xfId="216" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="331" hidden="1"/>
-    <cellStyle name="Hyperlink 101" xfId="666"/>
-    <cellStyle name="Hyperlink 102" xfId="217" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="332" hidden="1"/>
-    <cellStyle name="Hyperlink 102" xfId="667"/>
-    <cellStyle name="Hyperlink 103" xfId="218" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="333" hidden="1"/>
-    <cellStyle name="Hyperlink 103" xfId="668"/>
-    <cellStyle name="Hyperlink 104" xfId="219" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="334" hidden="1"/>
-    <cellStyle name="Hyperlink 104" xfId="669"/>
-    <cellStyle name="Hyperlink 105" xfId="220" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="335" hidden="1"/>
-    <cellStyle name="Hyperlink 105" xfId="670"/>
-    <cellStyle name="Hyperlink 106" xfId="221" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="336" hidden="1"/>
-    <cellStyle name="Hyperlink 106" xfId="671"/>
-    <cellStyle name="Hyperlink 107" xfId="222" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="337" hidden="1"/>
-    <cellStyle name="Hyperlink 107" xfId="672"/>
-    <cellStyle name="Hyperlink 108" xfId="223" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="338" hidden="1"/>
-    <cellStyle name="Hyperlink 108" xfId="673"/>
-    <cellStyle name="Hyperlink 109" xfId="224" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="339" hidden="1"/>
-    <cellStyle name="Hyperlink 109" xfId="674"/>
-    <cellStyle name="Hyperlink 11" xfId="126" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="279" hidden="1"/>
-    <cellStyle name="Hyperlink 11" xfId="614"/>
-    <cellStyle name="Hyperlink 110" xfId="225" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="340" hidden="1"/>
-    <cellStyle name="Hyperlink 110" xfId="675"/>
-    <cellStyle name="Hyperlink 111" xfId="226" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="341" hidden="1"/>
-    <cellStyle name="Hyperlink 111" xfId="676"/>
-    <cellStyle name="Hyperlink 112" xfId="555"/>
-    <cellStyle name="Hyperlink 113" xfId="115"/>
-    <cellStyle name="Hyperlink 12" xfId="127" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="278" hidden="1"/>
-    <cellStyle name="Hyperlink 12" xfId="613"/>
-    <cellStyle name="Hyperlink 13" xfId="128" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="277" hidden="1"/>
-    <cellStyle name="Hyperlink 13" xfId="612"/>
-    <cellStyle name="Hyperlink 14" xfId="129" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="276" hidden="1"/>
-    <cellStyle name="Hyperlink 14" xfId="68"/>
-    <cellStyle name="Hyperlink 15" xfId="130" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="275" hidden="1"/>
-    <cellStyle name="Hyperlink 15" xfId="69"/>
-    <cellStyle name="Hyperlink 16" xfId="131" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="274" hidden="1"/>
-    <cellStyle name="Hyperlink 16" xfId="70"/>
-    <cellStyle name="Hyperlink 17" xfId="132" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="273" hidden="1"/>
-    <cellStyle name="Hyperlink 17" xfId="71"/>
-    <cellStyle name="Hyperlink 18" xfId="133" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="272" hidden="1"/>
-    <cellStyle name="Hyperlink 18" xfId="72"/>
-    <cellStyle name="Hyperlink 19" xfId="134" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="271" hidden="1"/>
-    <cellStyle name="Hyperlink 19" xfId="73"/>
-    <cellStyle name="Hyperlink 2" xfId="9"/>
-    <cellStyle name="Hyperlink 2 2" xfId="480"/>
-    <cellStyle name="Hyperlink 2 3" xfId="116" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="228" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="288" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="342" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="113" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="623" hidden="1"/>
-    <cellStyle name="Hyperlink 2 3" xfId="677"/>
-    <cellStyle name="Hyperlink 20" xfId="135" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="270" hidden="1"/>
-    <cellStyle name="Hyperlink 20" xfId="74"/>
-    <cellStyle name="Hyperlink 21" xfId="136" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="269" hidden="1"/>
-    <cellStyle name="Hyperlink 21" xfId="75"/>
-    <cellStyle name="Hyperlink 22" xfId="137" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="268" hidden="1"/>
-    <cellStyle name="Hyperlink 22" xfId="76"/>
-    <cellStyle name="Hyperlink 23" xfId="138" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="267" hidden="1"/>
-    <cellStyle name="Hyperlink 23" xfId="77"/>
-    <cellStyle name="Hyperlink 24" xfId="139" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="266" hidden="1"/>
-    <cellStyle name="Hyperlink 24" xfId="78"/>
-    <cellStyle name="Hyperlink 25" xfId="140" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="265" hidden="1"/>
-    <cellStyle name="Hyperlink 25" xfId="79"/>
-    <cellStyle name="Hyperlink 26" xfId="141" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="264" hidden="1"/>
-    <cellStyle name="Hyperlink 26" xfId="80"/>
-    <cellStyle name="Hyperlink 27" xfId="142" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="263" hidden="1"/>
-    <cellStyle name="Hyperlink 27" xfId="81"/>
-    <cellStyle name="Hyperlink 28" xfId="143" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="262" hidden="1"/>
-    <cellStyle name="Hyperlink 28" xfId="82"/>
-    <cellStyle name="Hyperlink 29" xfId="144" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="261" hidden="1"/>
-    <cellStyle name="Hyperlink 29" xfId="83"/>
-    <cellStyle name="Hyperlink 3" xfId="118" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="287" hidden="1"/>
-    <cellStyle name="Hyperlink 3" xfId="622"/>
-    <cellStyle name="Hyperlink 30" xfId="145" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="260" hidden="1"/>
-    <cellStyle name="Hyperlink 30" xfId="84"/>
-    <cellStyle name="Hyperlink 31" xfId="146" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="259" hidden="1"/>
-    <cellStyle name="Hyperlink 31" xfId="85"/>
-    <cellStyle name="Hyperlink 32" xfId="147" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="258" hidden="1"/>
-    <cellStyle name="Hyperlink 32" xfId="86"/>
-    <cellStyle name="Hyperlink 33" xfId="148" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="257" hidden="1"/>
-    <cellStyle name="Hyperlink 33" xfId="87"/>
-    <cellStyle name="Hyperlink 34" xfId="149" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="256" hidden="1"/>
-    <cellStyle name="Hyperlink 34" xfId="88"/>
-    <cellStyle name="Hyperlink 35" xfId="150" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="255" hidden="1"/>
-    <cellStyle name="Hyperlink 35" xfId="89"/>
-    <cellStyle name="Hyperlink 36" xfId="151" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="254" hidden="1"/>
-    <cellStyle name="Hyperlink 36" xfId="90"/>
-    <cellStyle name="Hyperlink 37" xfId="152" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="253" hidden="1"/>
-    <cellStyle name="Hyperlink 37" xfId="91"/>
-    <cellStyle name="Hyperlink 38" xfId="153" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="252" hidden="1"/>
-    <cellStyle name="Hyperlink 38" xfId="92"/>
-    <cellStyle name="Hyperlink 39" xfId="154" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="251" hidden="1"/>
-    <cellStyle name="Hyperlink 39" xfId="93"/>
-    <cellStyle name="Hyperlink 4" xfId="119" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="286" hidden="1"/>
-    <cellStyle name="Hyperlink 4" xfId="621"/>
-    <cellStyle name="Hyperlink 40" xfId="155" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="250" hidden="1"/>
-    <cellStyle name="Hyperlink 40" xfId="94"/>
-    <cellStyle name="Hyperlink 41" xfId="156" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="249" hidden="1"/>
-    <cellStyle name="Hyperlink 41" xfId="95"/>
-    <cellStyle name="Hyperlink 42" xfId="157" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="248" hidden="1"/>
-    <cellStyle name="Hyperlink 42" xfId="96"/>
-    <cellStyle name="Hyperlink 43" xfId="158" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="247" hidden="1"/>
-    <cellStyle name="Hyperlink 43" xfId="97"/>
-    <cellStyle name="Hyperlink 44" xfId="159" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="246" hidden="1"/>
-    <cellStyle name="Hyperlink 44" xfId="98"/>
-    <cellStyle name="Hyperlink 45" xfId="160" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="245" hidden="1"/>
-    <cellStyle name="Hyperlink 45" xfId="99"/>
-    <cellStyle name="Hyperlink 46" xfId="161" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="244" hidden="1"/>
-    <cellStyle name="Hyperlink 46" xfId="100"/>
-    <cellStyle name="Hyperlink 47" xfId="162" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="243" hidden="1"/>
-    <cellStyle name="Hyperlink 47" xfId="101"/>
-    <cellStyle name="Hyperlink 48" xfId="163" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="242" hidden="1"/>
-    <cellStyle name="Hyperlink 48" xfId="102"/>
-    <cellStyle name="Hyperlink 49" xfId="164" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="241" hidden="1"/>
-    <cellStyle name="Hyperlink 49" xfId="103"/>
-    <cellStyle name="Hyperlink 5" xfId="120" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="285" hidden="1"/>
-    <cellStyle name="Hyperlink 5" xfId="620"/>
-    <cellStyle name="Hyperlink 50" xfId="165" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="240" hidden="1"/>
-    <cellStyle name="Hyperlink 50" xfId="104"/>
-    <cellStyle name="Hyperlink 51" xfId="166" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="239" hidden="1"/>
-    <cellStyle name="Hyperlink 51" xfId="105"/>
-    <cellStyle name="Hyperlink 52" xfId="167" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="238" hidden="1"/>
-    <cellStyle name="Hyperlink 52" xfId="106"/>
-    <cellStyle name="Hyperlink 53" xfId="168" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="237" hidden="1"/>
-    <cellStyle name="Hyperlink 53" xfId="107"/>
-    <cellStyle name="Hyperlink 54" xfId="169" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="236" hidden="1"/>
-    <cellStyle name="Hyperlink 54" xfId="108"/>
-    <cellStyle name="Hyperlink 55" xfId="170" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="235" hidden="1"/>
-    <cellStyle name="Hyperlink 55" xfId="109"/>
-    <cellStyle name="Hyperlink 56" xfId="171" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="234" hidden="1"/>
-    <cellStyle name="Hyperlink 56" xfId="110"/>
-    <cellStyle name="Hyperlink 57" xfId="172" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="233" hidden="1"/>
-    <cellStyle name="Hyperlink 57" xfId="111"/>
-    <cellStyle name="Hyperlink 58" xfId="173" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="289" hidden="1"/>
-    <cellStyle name="Hyperlink 58" xfId="624"/>
-    <cellStyle name="Hyperlink 59" xfId="174" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="232" hidden="1"/>
-    <cellStyle name="Hyperlink 59" xfId="112"/>
-    <cellStyle name="Hyperlink 6" xfId="121" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="284" hidden="1"/>
-    <cellStyle name="Hyperlink 6" xfId="619"/>
-    <cellStyle name="Hyperlink 60" xfId="175" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="290" hidden="1"/>
-    <cellStyle name="Hyperlink 60" xfId="625"/>
-    <cellStyle name="Hyperlink 61" xfId="176" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="291" hidden="1"/>
-    <cellStyle name="Hyperlink 61" xfId="626"/>
-    <cellStyle name="Hyperlink 62" xfId="177" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="292" hidden="1"/>
-    <cellStyle name="Hyperlink 62" xfId="627"/>
-    <cellStyle name="Hyperlink 63" xfId="178" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="293" hidden="1"/>
-    <cellStyle name="Hyperlink 63" xfId="628"/>
-    <cellStyle name="Hyperlink 64" xfId="179" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="294" hidden="1"/>
-    <cellStyle name="Hyperlink 64" xfId="629"/>
-    <cellStyle name="Hyperlink 65" xfId="180" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="295" hidden="1"/>
-    <cellStyle name="Hyperlink 65" xfId="630"/>
-    <cellStyle name="Hyperlink 66" xfId="181" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="296" hidden="1"/>
-    <cellStyle name="Hyperlink 66" xfId="631"/>
-    <cellStyle name="Hyperlink 67" xfId="182" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="297" hidden="1"/>
-    <cellStyle name="Hyperlink 67" xfId="632"/>
-    <cellStyle name="Hyperlink 68" xfId="183" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="298" hidden="1"/>
-    <cellStyle name="Hyperlink 68" xfId="633"/>
-    <cellStyle name="Hyperlink 69" xfId="184" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="299" hidden="1"/>
-    <cellStyle name="Hyperlink 69" xfId="634"/>
-    <cellStyle name="Hyperlink 7" xfId="122" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="283" hidden="1"/>
-    <cellStyle name="Hyperlink 7" xfId="618"/>
-    <cellStyle name="Hyperlink 70" xfId="185" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="300" hidden="1"/>
-    <cellStyle name="Hyperlink 70" xfId="635"/>
-    <cellStyle name="Hyperlink 71" xfId="186" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="301" hidden="1"/>
-    <cellStyle name="Hyperlink 71" xfId="636"/>
-    <cellStyle name="Hyperlink 72" xfId="187" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="302" hidden="1"/>
-    <cellStyle name="Hyperlink 72" xfId="637"/>
-    <cellStyle name="Hyperlink 73" xfId="188" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="303" hidden="1"/>
-    <cellStyle name="Hyperlink 73" xfId="638"/>
-    <cellStyle name="Hyperlink 74" xfId="189" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="304" hidden="1"/>
-    <cellStyle name="Hyperlink 74" xfId="639"/>
-    <cellStyle name="Hyperlink 75" xfId="190" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="305" hidden="1"/>
-    <cellStyle name="Hyperlink 75" xfId="640"/>
-    <cellStyle name="Hyperlink 76" xfId="191" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="306" hidden="1"/>
-    <cellStyle name="Hyperlink 76" xfId="641"/>
-    <cellStyle name="Hyperlink 77" xfId="192" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="307" hidden="1"/>
-    <cellStyle name="Hyperlink 77" xfId="642"/>
-    <cellStyle name="Hyperlink 78" xfId="193" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="308" hidden="1"/>
-    <cellStyle name="Hyperlink 78" xfId="643"/>
-    <cellStyle name="Hyperlink 79" xfId="194" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="309" hidden="1"/>
-    <cellStyle name="Hyperlink 79" xfId="644"/>
-    <cellStyle name="Hyperlink 8" xfId="123" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="282" hidden="1"/>
-    <cellStyle name="Hyperlink 8" xfId="617"/>
-    <cellStyle name="Hyperlink 80" xfId="195" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="310" hidden="1"/>
-    <cellStyle name="Hyperlink 80" xfId="645"/>
-    <cellStyle name="Hyperlink 81" xfId="196" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="311" hidden="1"/>
-    <cellStyle name="Hyperlink 81" xfId="646"/>
-    <cellStyle name="Hyperlink 82" xfId="197" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="312" hidden="1"/>
-    <cellStyle name="Hyperlink 82" xfId="647"/>
-    <cellStyle name="Hyperlink 83" xfId="198" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="313" hidden="1"/>
-    <cellStyle name="Hyperlink 83" xfId="648"/>
-    <cellStyle name="Hyperlink 84" xfId="199" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="314" hidden="1"/>
-    <cellStyle name="Hyperlink 84" xfId="649"/>
-    <cellStyle name="Hyperlink 85" xfId="200" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="315" hidden="1"/>
-    <cellStyle name="Hyperlink 85" xfId="650"/>
-    <cellStyle name="Hyperlink 86" xfId="201" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="316" hidden="1"/>
-    <cellStyle name="Hyperlink 86" xfId="651"/>
-    <cellStyle name="Hyperlink 87" xfId="202" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="317" hidden="1"/>
-    <cellStyle name="Hyperlink 87" xfId="652"/>
-    <cellStyle name="Hyperlink 88" xfId="203" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="318" hidden="1"/>
-    <cellStyle name="Hyperlink 88" xfId="653"/>
-    <cellStyle name="Hyperlink 89" xfId="204" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="319" hidden="1"/>
-    <cellStyle name="Hyperlink 89" xfId="654"/>
-    <cellStyle name="Hyperlink 9" xfId="124" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="281" hidden="1"/>
-    <cellStyle name="Hyperlink 9" xfId="616"/>
-    <cellStyle name="Hyperlink 90" xfId="205" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="320" hidden="1"/>
-    <cellStyle name="Hyperlink 90" xfId="655"/>
-    <cellStyle name="Hyperlink 91" xfId="206" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="321" hidden="1"/>
-    <cellStyle name="Hyperlink 91" xfId="656"/>
-    <cellStyle name="Hyperlink 92" xfId="207" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="322" hidden="1"/>
-    <cellStyle name="Hyperlink 92" xfId="657"/>
-    <cellStyle name="Hyperlink 93" xfId="208" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="323" hidden="1"/>
-    <cellStyle name="Hyperlink 93" xfId="658"/>
-    <cellStyle name="Hyperlink 94" xfId="209" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="324" hidden="1"/>
-    <cellStyle name="Hyperlink 94" xfId="659"/>
-    <cellStyle name="Hyperlink 95" xfId="210" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="325" hidden="1"/>
-    <cellStyle name="Hyperlink 95" xfId="660"/>
-    <cellStyle name="Hyperlink 96" xfId="211" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="326" hidden="1"/>
-    <cellStyle name="Hyperlink 96" xfId="661"/>
-    <cellStyle name="Hyperlink 97" xfId="212" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="327" hidden="1"/>
-    <cellStyle name="Hyperlink 97" xfId="662"/>
-    <cellStyle name="Hyperlink 98" xfId="213" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="328" hidden="1"/>
-    <cellStyle name="Hyperlink 98" xfId="663"/>
-    <cellStyle name="Hyperlink 99" xfId="214" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="329" hidden="1"/>
-    <cellStyle name="Hyperlink 99" xfId="664"/>
+    <cellStyle name="Heading 4 2" xfId="352" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Hed Side" xfId="14" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="58" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Hed Top" xfId="57" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="125" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="280" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Hyperlink 10" xfId="615" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="215" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="330" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Hyperlink 100" xfId="665" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="216" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="331" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Hyperlink 101" xfId="666" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="217" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="332" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Hyperlink 102" xfId="667" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="218" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="333" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Hyperlink 103" xfId="668" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="219" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="334" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Hyperlink 104" xfId="669" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="220" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="335" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Hyperlink 105" xfId="670" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="221" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="336" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Hyperlink 106" xfId="671" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="222" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="337" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Hyperlink 107" xfId="672" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="223" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="338" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Hyperlink 108" xfId="673" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="224" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="339" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Hyperlink 109" xfId="674" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="126" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="279" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="614" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="225" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="340" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Hyperlink 110" xfId="675" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="226" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="341" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Hyperlink 111" xfId="676" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Hyperlink 112" xfId="555" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Hyperlink 113" xfId="115" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="127" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="278" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Hyperlink 12" xfId="613" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="128" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="277" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Hyperlink 13" xfId="612" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="129" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="276" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Hyperlink 14" xfId="68" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="130" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="275" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Hyperlink 15" xfId="69" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="131" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="274" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="70" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Hyperlink 17" xfId="132" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Hyperlink 17" xfId="273" hidden="1" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Hyperlink 17" xfId="71" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="133" hidden="1" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="272" hidden="1" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Hyperlink 18" xfId="72" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="134" hidden="1" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="271" hidden="1" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Hyperlink 19" xfId="73" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="116" hidden="1" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="228" hidden="1" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="288" hidden="1" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="342" hidden="1" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="113" hidden="1" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="623" hidden="1" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="677" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="135" hidden="1" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="270" hidden="1" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Hyperlink 20" xfId="74" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="136" hidden="1" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="269" hidden="1" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Hyperlink 21" xfId="75" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="137" hidden="1" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="268" hidden="1" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Hyperlink 22" xfId="76" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="138" hidden="1" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="267" hidden="1" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Hyperlink 23" xfId="77" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="139" hidden="1" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="266" hidden="1" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Hyperlink 24" xfId="78" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="140" hidden="1" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="265" hidden="1" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Hyperlink 25" xfId="79" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="141" hidden="1" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="264" hidden="1" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Hyperlink 26" xfId="80" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="142" hidden="1" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="263" hidden="1" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Hyperlink 27" xfId="81" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="143" hidden="1" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="262" hidden="1" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Hyperlink 28" xfId="82" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="144" hidden="1" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="261" hidden="1" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Hyperlink 29" xfId="83" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="118" hidden="1" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="287" hidden="1" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="622" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="145" hidden="1" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="260" hidden="1" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Hyperlink 30" xfId="84" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="146" hidden="1" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="259" hidden="1" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Hyperlink 31" xfId="85" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="147" hidden="1" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="258" hidden="1" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Hyperlink 32" xfId="86" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="148" hidden="1" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="257" hidden="1" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Hyperlink 33" xfId="87" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="149" hidden="1" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="256" hidden="1" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Hyperlink 34" xfId="88" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="150" hidden="1" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="255" hidden="1" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Hyperlink 35" xfId="89" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="151" hidden="1" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="254" hidden="1" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Hyperlink 36" xfId="90" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="152" hidden="1" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="253" hidden="1" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Hyperlink 37" xfId="91" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="153" hidden="1" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="252" hidden="1" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Hyperlink 38" xfId="92" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="154" hidden="1" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="251" hidden="1" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Hyperlink 39" xfId="93" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="119" hidden="1" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="286" hidden="1" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="621" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="155" hidden="1" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="250" hidden="1" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Hyperlink 40" xfId="94" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="156" hidden="1" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="249" hidden="1" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Hyperlink 41" xfId="95" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="157" hidden="1" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="248" hidden="1" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Hyperlink 42" xfId="96" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="158" hidden="1" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="247" hidden="1" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Hyperlink 43" xfId="97" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="159" hidden="1" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="246" hidden="1" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Hyperlink 44" xfId="98" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="160" hidden="1" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="245" hidden="1" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Hyperlink 45" xfId="99" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="161" hidden="1" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="244" hidden="1" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Hyperlink 46" xfId="100" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="162" hidden="1" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="243" hidden="1" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Hyperlink 47" xfId="101" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="163" hidden="1" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="242" hidden="1" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Hyperlink 48" xfId="102" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="164" hidden="1" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="241" hidden="1" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Hyperlink 49" xfId="103" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="120" hidden="1" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="285" hidden="1" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="620" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="165" hidden="1" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="240" hidden="1" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Hyperlink 50" xfId="104" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="166" hidden="1" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="239" hidden="1" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Hyperlink 51" xfId="105" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="167" hidden="1" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="238" hidden="1" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Hyperlink 52" xfId="106" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="168" hidden="1" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="237" hidden="1" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Hyperlink 53" xfId="107" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="169" hidden="1" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="236" hidden="1" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Hyperlink 54" xfId="108" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="170" hidden="1" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="235" hidden="1" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Hyperlink 55" xfId="109" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="171" hidden="1" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="234" hidden="1" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Hyperlink 56" xfId="110" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="172" hidden="1" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="233" hidden="1" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Hyperlink 57" xfId="111" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="173" hidden="1" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="289" hidden="1" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Hyperlink 58" xfId="624" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="174" hidden="1" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="232" hidden="1" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Hyperlink 59" xfId="112" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="121" hidden="1" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="284" hidden="1" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="619" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="175" hidden="1" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="290" hidden="1" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Hyperlink 60" xfId="625" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="176" hidden="1" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="291" hidden="1" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Hyperlink 61" xfId="626" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="177" hidden="1" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="292" hidden="1" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Hyperlink 62" xfId="627" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="178" hidden="1" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="293" hidden="1" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Hyperlink 63" xfId="628" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="179" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="294" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Hyperlink 64" xfId="629" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="180" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="295" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Hyperlink 65" xfId="630" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="181" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="296" hidden="1" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Hyperlink 66" xfId="631" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="182" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="297" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Hyperlink 67" xfId="632" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="183" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="298" hidden="1" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Hyperlink 68" xfId="633" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="184" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="299" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Hyperlink 69" xfId="634" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="122" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="283" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="618" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="185" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="300" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Hyperlink 70" xfId="635" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="186" hidden="1" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="301" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Hyperlink 71" xfId="636" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="187" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="302" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Hyperlink 72" xfId="637" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="188" hidden="1" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="303" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Hyperlink 73" xfId="638" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="189" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="304" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Hyperlink 74" xfId="639" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="190" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="305" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Hyperlink 75" xfId="640" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="191" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="306" hidden="1" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Hyperlink 76" xfId="641" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="192" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="307" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Hyperlink 77" xfId="642" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="193" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="308" hidden="1" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Hyperlink 78" xfId="643" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="194" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="309" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Hyperlink 79" xfId="644" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="123" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="282" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="195" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="310" hidden="1" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Hyperlink 80" xfId="645" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="196" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="311" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Hyperlink 81" xfId="646" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="197" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="312" hidden="1" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Hyperlink 82" xfId="647" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="198" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="313" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Hyperlink 83" xfId="648" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="199" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="314" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Hyperlink 84" xfId="649" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="200" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="315" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Hyperlink 85" xfId="650" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="201" hidden="1" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="316" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Hyperlink 86" xfId="651" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="202" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="317" hidden="1" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Hyperlink 87" xfId="652" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="203" hidden="1" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="318" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Hyperlink 88" xfId="653" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="204" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="319" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Hyperlink 89" xfId="654" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="124" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="281" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Hyperlink 9" xfId="616" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="205" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="320" hidden="1" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Hyperlink 90" xfId="655" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="206" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="321" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Hyperlink 91" xfId="656" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="207" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="322" hidden="1" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Hyperlink 92" xfId="657" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="208" hidden="1" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="323" hidden="1" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Hyperlink 93" xfId="658" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="209" hidden="1" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="324" hidden="1" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Hyperlink 94" xfId="659" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="210" hidden="1" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="325" hidden="1" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Hyperlink 95" xfId="660" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="211" hidden="1" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="326" hidden="1" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Hyperlink 96" xfId="661" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="212" hidden="1" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="327" hidden="1" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Hyperlink 97" xfId="662" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="213" hidden="1" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="328" hidden="1" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Hyperlink 98" xfId="663" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="214" hidden="1" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="329" hidden="1" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Hyperlink 99" xfId="664" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
     <cellStyle name="Input" xfId="23" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input [yellow]" xfId="481"/>
-    <cellStyle name="Input [yellow] 2" xfId="482"/>
-    <cellStyle name="Input [yellow] 2 2" xfId="688"/>
-    <cellStyle name="Input [yellow] 3" xfId="483"/>
-    <cellStyle name="Input [yellow] 3 2" xfId="689"/>
-    <cellStyle name="Input [yellow] 4" xfId="687"/>
-    <cellStyle name="Input 2" xfId="63"/>
-    <cellStyle name="Input 3" xfId="574"/>
-    <cellStyle name="ITEMS" xfId="484"/>
+    <cellStyle name="Input [yellow]" xfId="481" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Input [yellow] 2" xfId="482" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Input [yellow] 2 2" xfId="688" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Input [yellow] 3" xfId="483" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Input [yellow] 3 2" xfId="689" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Input [yellow] 4" xfId="687" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Input 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Input 3" xfId="574" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="ITEMS" xfId="484" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
     <cellStyle name="Linked Cell" xfId="26" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Linked Cell 2" xfId="357"/>
-    <cellStyle name="m1 - Style1" xfId="485"/>
-    <cellStyle name="MANKAD" xfId="486"/>
+    <cellStyle name="Linked Cell 2" xfId="357" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="m1 - Style1" xfId="485" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="MANKAD" xfId="486" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
     <cellStyle name="Neutral" xfId="22" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="354"/>
-    <cellStyle name="Neutrale" xfId="487"/>
-    <cellStyle name="no dec" xfId="488"/>
+    <cellStyle name="Neutral 2" xfId="354" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Neutrale" xfId="487" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="no dec" xfId="488" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="489"/>
-    <cellStyle name="Normal 10" xfId="490"/>
-    <cellStyle name="Normal 11" xfId="419"/>
-    <cellStyle name="Normal 12" xfId="566"/>
-    <cellStyle name="Normal 13" xfId="572"/>
-    <cellStyle name="Normal 14" xfId="577"/>
-    <cellStyle name="Normal 14 2" xfId="580"/>
-    <cellStyle name="Normal 14 3" xfId="593"/>
-    <cellStyle name="Normal 14 3 2" xfId="600"/>
-    <cellStyle name="Normal 14 3 2 2" xfId="604"/>
-    <cellStyle name="Normal 14 3 2 2 2" xfId="607"/>
-    <cellStyle name="Normal 14 4" xfId="595"/>
-    <cellStyle name="Normal 14 4 2" xfId="597"/>
-    <cellStyle name="Normal 14 4 2 2" xfId="601"/>
-    <cellStyle name="Normal 14 4 2 2 2" xfId="605"/>
-    <cellStyle name="Normal 15" xfId="588"/>
-    <cellStyle name="Normal 16" xfId="609"/>
-    <cellStyle name="Normal 17" xfId="610"/>
-    <cellStyle name="Normal 18" xfId="60"/>
-    <cellStyle name="Normal 19" xfId="576"/>
-    <cellStyle name="Normal 2" xfId="66"/>
-    <cellStyle name="Normal 2 2" xfId="231"/>
-    <cellStyle name="Normal 2 2 2" xfId="346"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="492"/>
-    <cellStyle name="Normal 2 2 3" xfId="493"/>
-    <cellStyle name="Normal 2 2 4" xfId="491"/>
-    <cellStyle name="Normal 2 3" xfId="494"/>
-    <cellStyle name="Normal 3" xfId="229"/>
-    <cellStyle name="Normal 3 2" xfId="345"/>
-    <cellStyle name="Normal 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 3 3" xfId="497"/>
-    <cellStyle name="Normal 3 4" xfId="495"/>
-    <cellStyle name="Normal 4" xfId="383"/>
-    <cellStyle name="Normal 4 2" xfId="499"/>
-    <cellStyle name="Normal 4 3" xfId="498"/>
-    <cellStyle name="Normal 5" xfId="387"/>
-    <cellStyle name="Normal 5 2" xfId="500"/>
-    <cellStyle name="Normal 6" xfId="401"/>
-    <cellStyle name="Normal 6 2" xfId="501"/>
-    <cellStyle name="Normal 7" xfId="415"/>
-    <cellStyle name="Normal 7 2" xfId="417"/>
-    <cellStyle name="Normal 7 3" xfId="502"/>
-    <cellStyle name="Normal 7 3 2" xfId="564"/>
-    <cellStyle name="Normal 7 3 2 2" xfId="570"/>
-    <cellStyle name="Normal 8" xfId="503"/>
-    <cellStyle name="Normal 8 2" xfId="504"/>
-    <cellStyle name="Normal 8 2 2" xfId="560"/>
-    <cellStyle name="Normal 8 3" xfId="561"/>
-    <cellStyle name="Normal 8 3 2" xfId="591"/>
-    <cellStyle name="Normal 8 3 2 2" xfId="608"/>
-    <cellStyle name="Normal 9" xfId="505"/>
-    <cellStyle name="Normal 9 2" xfId="558"/>
-    <cellStyle name="Normal 9 3" xfId="565"/>
-    <cellStyle name="Normal 9 4" xfId="568"/>
-    <cellStyle name="Normal 9 5" xfId="569"/>
-    <cellStyle name="Normal 9 6" xfId="571"/>
-    <cellStyle name="Normal 9 6 2" xfId="592"/>
-    <cellStyle name="Normal 9 6 2 2" xfId="611"/>
-    <cellStyle name="Nota" xfId="506"/>
-    <cellStyle name="Nota 2" xfId="507"/>
-    <cellStyle name="Nota 2 2" xfId="691"/>
-    <cellStyle name="Nota 3" xfId="508"/>
-    <cellStyle name="Nota 3 2" xfId="692"/>
-    <cellStyle name="Nota 4" xfId="690"/>
+    <cellStyle name="Normal - Style1" xfId="489" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 10" xfId="490" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 11" xfId="419" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 12" xfId="566" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 13" xfId="572" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 14" xfId="577" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 14 2" xfId="580" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 14 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 14 3 2" xfId="600" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 14 3 2 2" xfId="604" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 14 3 2 2 2" xfId="607" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 14 4" xfId="595" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 14 4 2" xfId="597" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 14 4 2 2" xfId="601" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 14 4 2 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 15" xfId="588" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 16" xfId="609" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 17" xfId="610" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 18" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 19" xfId="576" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 2" xfId="66" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 2 2" xfId="231" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="346" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="492" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="493" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="491" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 2 3" xfId="494" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 3" xfId="229" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 3 2" xfId="345" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 3 3" xfId="497" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 4" xfId="383" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 4 2" xfId="499" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 4 3" xfId="498" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 5" xfId="387" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 5 2" xfId="500" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6" xfId="401" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 2" xfId="501" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 7" xfId="415" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 7 2" xfId="417" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 7 3" xfId="502" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 7 3 2" xfId="564" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 7 3 2 2" xfId="570" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 8" xfId="503" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 8 2" xfId="504" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 8 3" xfId="561" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 8 3 2" xfId="591" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 8 3 2 2" xfId="608" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 9" xfId="505" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 9 2" xfId="558" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 9 3" xfId="565" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 9 4" xfId="568" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 9 5" xfId="569" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 9 6" xfId="571" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 9 6 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 9 6 2 2" xfId="611" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Nota" xfId="506" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Nota 2" xfId="507" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Nota 2 2" xfId="691" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Nota 3" xfId="508" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Nota 3 2" xfId="692" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Nota 4" xfId="690" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
     <cellStyle name="Note" xfId="29" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="384"/>
-    <cellStyle name="Note 3" xfId="388"/>
-    <cellStyle name="Note 4" xfId="402"/>
-    <cellStyle name="Num0 - Style7" xfId="509"/>
-    <cellStyle name="Num2 - Style8" xfId="510"/>
-    <cellStyle name="Numeri - Style1" xfId="511"/>
-    <cellStyle name="Numeri - Style1 2" xfId="512"/>
-    <cellStyle name="Numeri - Style1 2 2" xfId="694"/>
-    <cellStyle name="Numeri - Style1 3" xfId="693"/>
-    <cellStyle name="ofwhich" xfId="64"/>
+    <cellStyle name="Note 2" xfId="384" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Note 3" xfId="388" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Note 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Num0 - Style7" xfId="509" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Num2 - Style8" xfId="510" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Numeri - Style1" xfId="511" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Numeri - Style1 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Numeri - Style1 2 2" xfId="694" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Numeri - Style1 3" xfId="693" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="ofwhich" xfId="64" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
     <cellStyle name="Output" xfId="24" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="355"/>
-    <cellStyle name="Parent row" xfId="5"/>
-    <cellStyle name="Percent [2]" xfId="513"/>
-    <cellStyle name="Percent 10" xfId="575"/>
-    <cellStyle name="Percent 2" xfId="67"/>
-    <cellStyle name="Percent 2 2" xfId="423"/>
-    <cellStyle name="Percent 3" xfId="514"/>
-    <cellStyle name="Percent 3 2" xfId="515"/>
-    <cellStyle name="Percent 3 3" xfId="516"/>
-    <cellStyle name="Percent 3 4" xfId="563"/>
-    <cellStyle name="Percent 4" xfId="517"/>
-    <cellStyle name="Percent 4 2" xfId="518"/>
-    <cellStyle name="Percent 5" xfId="519"/>
-    <cellStyle name="Percent 6" xfId="421"/>
-    <cellStyle name="Percent 7" xfId="567"/>
-    <cellStyle name="Percent 8" xfId="585"/>
-    <cellStyle name="Percent 8 2" xfId="594"/>
-    <cellStyle name="Percent 8 3" xfId="596"/>
-    <cellStyle name="Percent 8 3 2" xfId="599"/>
-    <cellStyle name="Percent 8 3 2 2" xfId="603"/>
-    <cellStyle name="Percent 8 3 2 2 2" xfId="606"/>
-    <cellStyle name="Percent 9" xfId="61"/>
-    <cellStyle name="RevList" xfId="520"/>
-    <cellStyle name="Row headings" xfId="521"/>
-    <cellStyle name="Row headings Level 1" xfId="522"/>
-    <cellStyle name="Row headings Level 2" xfId="523"/>
-    <cellStyle name="Section Break" xfId="7"/>
-    <cellStyle name="Section Break: parent row" xfId="4"/>
-    <cellStyle name="Source - Style2" xfId="524"/>
-    <cellStyle name="Sources list" xfId="525"/>
-    <cellStyle name="Sources list 2" xfId="526"/>
-    <cellStyle name="Sources Title" xfId="527"/>
-    <cellStyle name="Sources Title 2" xfId="528"/>
-    <cellStyle name="style" xfId="529"/>
-    <cellStyle name="style 2" xfId="530"/>
-    <cellStyle name="style 2 2" xfId="696"/>
-    <cellStyle name="style 3" xfId="531"/>
-    <cellStyle name="style 3 2" xfId="697"/>
-    <cellStyle name="style 4" xfId="695"/>
-    <cellStyle name="style1" xfId="532"/>
-    <cellStyle name="style2" xfId="533"/>
-    <cellStyle name="Subtotal" xfId="534"/>
-    <cellStyle name="Table  - Style3" xfId="535"/>
-    <cellStyle name="Table  - Style4" xfId="536"/>
-    <cellStyle name="Table  - Style4 2" xfId="537"/>
-    <cellStyle name="Table  - Style6" xfId="538"/>
-    <cellStyle name="Table  - Style6 2" xfId="539"/>
-    <cellStyle name="Table no" xfId="540"/>
-    <cellStyle name="Table title" xfId="12"/>
-    <cellStyle name="Table_HeaderRow" xfId="65"/>
-    <cellStyle name="Testo avviso" xfId="541"/>
-    <cellStyle name="Testo descrittivo" xfId="542"/>
-    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="543"/>
-    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="544"/>
+    <cellStyle name="Output 2" xfId="355" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Percent [2]" xfId="513" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Percent 10" xfId="575" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Percent 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Percent 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Percent 3" xfId="514" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Percent 3 2" xfId="515" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Percent 3 3" xfId="516" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Percent 3 4" xfId="563" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Percent 4" xfId="517" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Percent 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Percent 5" xfId="519" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Percent 6" xfId="421" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Percent 7" xfId="567" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Percent 8" xfId="585" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Percent 8 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Percent 8 3" xfId="596" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Percent 8 3 2" xfId="599" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Percent 8 3 2 2" xfId="603" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Percent 8 3 2 2 2" xfId="606" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Percent 9" xfId="61" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="RevList" xfId="520" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Row headings" xfId="521" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Row headings Level 1" xfId="522" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Row headings Level 2" xfId="523" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Section Break" xfId="7" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Section Break: parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Source - Style2" xfId="524" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Sources list" xfId="525" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Sources list 2" xfId="526" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Sources Title" xfId="527" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Sources Title 2" xfId="528" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="style" xfId="529" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="style 2" xfId="530" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
+    <cellStyle name="style 2 2" xfId="696" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
+    <cellStyle name="style 3" xfId="531" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
+    <cellStyle name="style 3 2" xfId="697" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
+    <cellStyle name="style 4" xfId="695" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
+    <cellStyle name="style1" xfId="532" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
+    <cellStyle name="style2" xfId="533" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
+    <cellStyle name="Subtotal" xfId="534" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
+    <cellStyle name="Table  - Style3" xfId="535" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
+    <cellStyle name="Table  - Style4" xfId="536" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
+    <cellStyle name="Table  - Style4 2" xfId="537" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
+    <cellStyle name="Table  - Style6" xfId="538" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
+    <cellStyle name="Table  - Style6 2" xfId="539" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
+    <cellStyle name="Table no" xfId="540" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
+    <cellStyle name="Table title" xfId="12" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
+    <cellStyle name="Table_HeaderRow" xfId="65" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
+    <cellStyle name="Testo avviso" xfId="541" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
+    <cellStyle name="Testo descrittivo" xfId="542" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
+    <cellStyle name="þ_x001d_ð &amp;ý&amp;†ýG_x0008_ X_x000a__x0007__x0001__x0001_" xfId="543" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
+    <cellStyle name="þ_x001d_ð&quot;_x000c_Býò_x000c_5ýU_x0001_e_x0005_¹,_x0007__x0001__x0001_" xfId="544" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
     <cellStyle name="Title" xfId="15" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title-2" xfId="56"/>
-    <cellStyle name="Titolo" xfId="545"/>
-    <cellStyle name="Titolo 1" xfId="546"/>
-    <cellStyle name="Titolo 2" xfId="547"/>
-    <cellStyle name="Titolo 3" xfId="548"/>
-    <cellStyle name="Titolo 4" xfId="549"/>
+    <cellStyle name="Title-2" xfId="56" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
+    <cellStyle name="Titolo" xfId="545" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
+    <cellStyle name="Titolo 1" xfId="546" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
+    <cellStyle name="Titolo 2" xfId="547" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
+    <cellStyle name="Titolo 3" xfId="548" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
+    <cellStyle name="Titolo 4" xfId="549" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
     <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="361"/>
-    <cellStyle name="Totale" xfId="550"/>
-    <cellStyle name="Totale 2" xfId="551"/>
-    <cellStyle name="Totale 2 2" xfId="699"/>
-    <cellStyle name="Totale 3" xfId="552"/>
-    <cellStyle name="Totale 3 2" xfId="700"/>
-    <cellStyle name="Totale 4" xfId="698"/>
-    <cellStyle name="Valore non valido" xfId="553"/>
-    <cellStyle name="Valore valido" xfId="554"/>
+    <cellStyle name="Total 2" xfId="361" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
+    <cellStyle name="Totale" xfId="550" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
+    <cellStyle name="Totale 2" xfId="551" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
+    <cellStyle name="Totale 2 2" xfId="699" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
+    <cellStyle name="Totale 3" xfId="552" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
+    <cellStyle name="Totale 3 2" xfId="700" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
+    <cellStyle name="Totale 4" xfId="698" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
+    <cellStyle name="Valore non valido" xfId="553" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
+    <cellStyle name="Valore valido" xfId="554" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
     <cellStyle name="Warning Text" xfId="28" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Warning Text 2" xfId="359"/>
+    <cellStyle name="Warning Text 2" xfId="359" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -3553,17 +3561,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
-    <tableStyle name="EnergyCalcTables" pivot="0" count="4">
+    <tableStyle name="EnergyCalcTables" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0"/>
+    <tableStyle name="EnergyCalcTables 2" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3652,6 +3660,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3687,6 +3712,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3862,16 +3904,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="132.265625" customWidth="1"/>
+    <col min="2" max="2" width="132.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3941,6 +3983,11 @@
     <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3950,21 +3997,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1328125" customWidth="1"/>
-    <col min="15" max="15" width="14.73046875" customWidth="1"/>
-    <col min="16" max="16" width="19.73046875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1">
@@ -3984,10 +4031,10 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>60</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -3997,533 +4044,533 @@
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>7.3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="J3" s="40" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="16"/>
+      <c r="J3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="37"/>
+      <c r="K3" s="36"/>
       <c r="M3" s="3">
         <v>5.3</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="23"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="17"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="16"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="38"/>
+      <c r="K4" s="37"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="23"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="40">
         <f>AVERAGE(G12:G17)</f>
         <v>18.333333333333332</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="37"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="23"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="25">
+      <c r="F6" s="20"/>
+      <c r="G6" s="24">
         <v>10</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="37"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="O6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="Q6" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="21" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="25">
+      <c r="F7" s="20"/>
+      <c r="G7" s="24">
         <v>10</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="40">
         <f>AVERAGE(G27:G30)</f>
         <v>9</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="37"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29" t="s">
+      <c r="N7" s="27"/>
+      <c r="O7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="Q7" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="23"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="21" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="25">
+      <c r="F8" s="20"/>
+      <c r="G8" s="24">
         <v>10</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="37"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="28" t="s">
+      <c r="N8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29" t="s">
+      <c r="O8" s="28"/>
+      <c r="P8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q8" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="21" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="25">
+      <c r="F9" s="20"/>
+      <c r="G9" s="24">
         <v>10</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="41">
         <f>(J5*G41+J7*G44)/SUM(G41,G44)</f>
         <v>16.402434831574382</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="37">
         <f>Q7</f>
         <v>10</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29" t="s">
+      <c r="N9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="Q9" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="16" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="25">
+      <c r="F10" s="20"/>
+      <c r="G10" s="24">
         <v>10</v>
       </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33" t="s">
+      <c r="O10" s="32"/>
+      <c r="P10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="34">
+      <c r="Q10" s="33">
         <v>31.877221924034789</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="21" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="25">
+      <c r="F11" s="20"/>
+      <c r="G11" s="24">
         <v>10</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="16" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="25">
+      <c r="F12" s="20"/>
+      <c r="G12" s="24">
         <v>20</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="37"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="23"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="21" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25">
+      <c r="F13" s="20"/>
+      <c r="G13" s="24">
         <v>20</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="40">
         <v>10</v>
       </c>
-      <c r="K13" s="38"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="23"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="21" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="25">
+      <c r="F14" s="20"/>
+      <c r="G14" s="24">
         <v>20</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="38"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="23"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="21" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="25">
+      <c r="F15" s="20"/>
+      <c r="G15" s="24">
         <v>20</v>
       </c>
-      <c r="J15" s="41">
+      <c r="J15" s="40">
         <v>10</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="37"/>
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="23"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="21" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="25">
+      <c r="F16" s="20"/>
+      <c r="G16" s="24">
         <v>15</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="37"/>
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="21" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="25">
+      <c r="F17" s="20"/>
+      <c r="G17" s="24">
         <v>15</v>
       </c>
-      <c r="J17" s="42">
+      <c r="J17" s="41">
         <f>AVERAGE(J13:J15)</f>
         <v>10</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="37">
         <f>Q6</f>
         <v>10</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="23"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="16" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="25">
+      <c r="F18" s="20"/>
+      <c r="G18" s="24">
         <v>12</v>
       </c>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="23"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="21" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="25">
+      <c r="F19" s="20"/>
+      <c r="G19" s="24">
         <v>12</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="43"/>
+      <c r="K19" s="42"/>
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="23"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="21" t="s">
+      <c r="A20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="25">
+      <c r="F20" s="20"/>
+      <c r="G20" s="24">
         <v>12</v>
       </c>
-      <c r="J20" s="38" t="s">
+      <c r="J20" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="38"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="23"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="21" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="25">
+      <c r="F21" s="20"/>
+      <c r="G21" s="24">
         <v>12</v>
       </c>
-      <c r="J21" s="38">
+      <c r="J21" s="37">
         <v>20</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="43">
         <f>Q10</f>
         <v>31.877221924034789</v>
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="23"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="16" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="25">
+      <c r="F22" s="20"/>
+      <c r="G22" s="24">
         <v>8</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="23"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="21" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="25">
+      <c r="F23" s="20"/>
+      <c r="G23" s="24">
         <v>8</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="43"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="23"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="21" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="25">
+      <c r="F24" s="20"/>
+      <c r="G24" s="24">
         <v>8</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J24" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="38"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="23"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="21" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="25">
+      <c r="F25" s="20"/>
+      <c r="G25" s="24">
         <v>8</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J25" s="37">
         <v>35</v>
       </c>
-      <c r="K25" s="38">
+      <c r="K25" s="37">
         <f>Q9</f>
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="23"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="21" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="25">
+      <c r="F26" s="20"/>
+      <c r="G26" s="24">
         <v>5</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="23"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="16" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="25">
+      <c r="F27" s="20"/>
+      <c r="G27" s="24">
         <v>8</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -4532,15 +4579,15 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="23"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="21" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="26">
+      <c r="F28" s="20"/>
+      <c r="G28" s="25">
         <v>8</v>
       </c>
       <c r="J28" t="s">
@@ -4548,32 +4595,32 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="23"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="21" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="26">
+      <c r="F29" s="20"/>
+      <c r="G29" s="25">
         <v>8</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <f>AVERAGE(G18:G21)</f>
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="23"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="21" t="s">
+      <c r="A30" s="22"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="26">
+      <c r="F30" s="20"/>
+      <c r="G30" s="25">
         <v>12</v>
       </c>
       <c r="J30" t="s">
@@ -4581,36 +4628,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="23"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="15" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="27">
+      <c r="F31" s="20"/>
+      <c r="G31" s="26">
         <v>35</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="10">
         <f>AVERAGE(G22:G26)</f>
         <v>7.4</v>
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="23"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="21" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="27">
+      <c r="F32" s="20"/>
+      <c r="G32" s="26">
         <v>35</v>
       </c>
       <c r="J32" t="s">
@@ -4618,28 +4665,28 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="23"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="13" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="24">
+      <c r="F33" s="13"/>
+      <c r="G33" s="23">
         <v>20</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="9">
         <f>AVERAGE(J29:J31)</f>
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15">
-      <c r="B36" s="45" t="s">
+    <row r="36" spans="1:14" ht="15.75">
+      <c r="B36" s="44" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4927,25 +4974,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:3" ht="45">
+      <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -4960,8 +5007,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="8">
-        <f>('India Data'!J9)</f>
-        <v>16.402434831574382</v>
+        <f>'India Data'!J5</f>
+        <v>18.333333333333332</v>
       </c>
       <c r="C2">
         <f>'India Data'!K9</f>
@@ -5011,11 +5058,11 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <f>B6</f>
+      <c r="B6" s="46">
+        <f>'India Data'!J7</f>
+        <v>9</v>
+      </c>
+      <c r="C6" s="45">
         <v>33</v>
       </c>
     </row>

</xml_diff>